<commit_message>
Move in dupe etecting logic
</commit_message>
<xml_diff>
--- a/outputs/basic-processing/basic-exclusions/psycinfo-exclusions.xlsx
+++ b/outputs/basic-processing/basic-exclusions/psycinfo-exclusions.xlsx
@@ -544,12 +544,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Malm, Heli;Sourander, Andre;Gissler, Mika;Gyllenberg, David;Hinkka-Yli-Salomäki, Susanna;McKeague, Ian, W.;Artama, Miia;Brown, Alan, S.</t>
+          <t>Malm, Heli;Sourander, Andre;Gissler, Mika;Gyllenberg, David;Hinkka-Yli-Salomaki, Susanna;McKeague, Ian, W.;Artama, Miia;Brown, Alan, S.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Objective: Using national register data, the authors examined the relationship between prenatal selective serotonin reuptake inhibitor (SSRI) treatment and pregnancy complications, accounting for psychiatric diagnoses related to SSRI use. Method: This was a population-based prospective birth cohort study using national register data. The sampling frame included 845,345 offspring, representing all singleton live births in Finland between 1996 and 2010. Pregnancies were classified as exposed to SSRIs (N = 15,729), unexposed to SSRIs but with psychiatric diagnoses (N = 9,652), and unexposed to medications and psychiatric diagnoses (N = 31,394). Pregnancy outcomes in SSRI users were compared with those in the unexposed groups. Results: Offspring of mothers who received SSRI prescriptions during pregnancy had a lower risk for late preterm birth (odds ratio = 0.84, 95% CI = 0.74–0.96), for very preterm birth (odds ratio = 0.52, 95% CI = 0.37–0.74), and for cesarean section (odds ratio = 0.70, 95% CI = 0.6620.75) compared with offspring of mothers unexposed to medications but with psychiatric disorders. In contrast, in SSRI-treated mothers, the risk was higher for offspring neonatal complications, including low Apgar score (odds ratio = 1.68, 95% CI = 1.34–2.12) and monitoring in a neonatal care unit (odds ratio = 1.24, 95% CI = 1.14–1.35). Compared with offspring of unexposed mothers, offspring of SSRI-treated mothers and mothers unexposed to medications but with psychiatric disorders were both at increased risk of many adverse pregnancy outcomes, including cesarean section and need for monitoring in a neonatal care unit. Conclusions: In a large national birth cohort, treatment of maternal psychiatric disorders with SSRIs during pregnancy was related to a lower risk of preterm birth and cesarean section but a higher risk of neonatal maladaptation. The findings provide novel evidence for a protective role of SSRIs on some deleterious reproductive outcomes, possibly by reducing maternal depressive symptoms. The divergent findings suggest that clinical decisions on SSRI use during pregnancy should be individualized, taking into account the mother’s psychiatric and reproductive history. (PsycINFO Database Record (c) 2016 APA, all rights reserved)</t>
+          <t>Objective: Using national register data, the authors examined the relationship between prenatal selective serotonin reuptake inhibitor (SSRI) treatment and pregnancy complications, accounting for psychiatric diagnoses related to SSRI use. Method: This was a population-based prospective birth cohort study using national register data. The sampling frame included 845,345 offspring, representing all singleton live births in Finland between 1996 and 2010. Pregnancies were classified as exposed to SSRIs (N = 15,729), unexposed to SSRIs but with psychiatric diagnoses (N = 9,652), and unexposed to medications and psychiatric diagnoses (N = 31,394). Pregnancy outcomes in SSRI users were compared with those in the unexposed groups. Results: Offspring of mothers who received SSRI prescriptions during pregnancy had a lower risk for late preterm birth (odds ratio = 0.84, 95% CI = 0.74-0.96), for very preterm birth (odds ratio = 0.52, 95% CI = 0.37-0.74), and for cesarean section (odds ratio = 0.70, 95% CI = 0.6620.75) compared with offspring of mothers unexposed to medications but with psychiatric disorders. In contrast, in SSRI-treated mothers, the risk was higher for offspring neonatal complications, including low Apgar score (odds ratio = 1.68, 95% CI = 1.34-2.12) and monitoring in a neonatal care unit (odds ratio = 1.24, 95% CI = 1.14-1.35). Compared with offspring of unexposed mothers, offspring of SSRI-treated mothers and mothers unexposed to medications but with psychiatric disorders were both at increased risk of many adverse pregnancy outcomes, including cesarean section and need for monitoring in a neonatal care unit. Conclusions: In a large national birth cohort, treatment of maternal psychiatric disorders with SSRIs during pregnancy was related to a lower risk of preterm birth and cesarean section but a higher risk of neonatal maladaptation. The findings provide novel evidence for a protective role of SSRIs on some deleterious reproductive outcomes, possibly by reducing maternal depressive symptoms. The divergent findings suggest that clinical decisions on SSRI use during pregnancy should be individualized, taking into account the mother's psychiatric and reproductive history. (PsycINFO Database Record (c) 2016 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -587,7 +587,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>pregnancy complications following prenatal exposure to ssris or maternal psychiatric disorders: results from population-based national register data;2015;malm</t>
+          <t>pregnancycomplicationsfollowingprenatalexposuretossrisormaternalpsychiatricdisorders:resultsfrompopulation-basednationalregisterdata;2015;malm</t>
         </is>
       </c>
     </row>
@@ -2052,12 +2052,12 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>a quasi-experimental effectiveness evaluation of the ’incredible years toddler’ parenting programme on children’s development aged 5: a study protocol;2023;mooney</t>
+          <t>aquasi-experimentaleffectivenessevaluationofthe'incredibleyearstoddler'parentingprogrammeonchildren'sdevelopmentaged5:astudyprotocol;2023;mooney</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a quasi-experimental effectiveness evaluation of the ’incredible years toddler’ parenting programme on children’s development aged 5: a study protocol</t>
+          <t>a quasi-experimental effectiveness evaluation of the 'incredible years toddler' parenting programme on children's development aged 5: a study protocol</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -2070,7 +2070,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Child behavioural and mental health problems have become a public health crisis. The consequences of poor mental health in childhood have large economic costs and consequences for the individual, their families, and for society. Early intervention through parenting programmes can reduce the onset of poor mental health in childhood, hence evaluating the effectiveness of parenting programmes is critical. The ‘Incredible Years Toddler’ parent programme is an education and training intervention designed to enhance the social and emotional wellbeing of children aged 1–3 years. Whilst previous studies show Incredible Years Toddler to provide promising effects on child outcomes in the short term, the research samples have lacked ethnic diversity and representation from socioeconomically deprived families. This quasi-experimental study is registered on ISRCTN (ISRCTN49991769). We will investigate the effectiveness of Incredible Years Toddler being delivered in three neighbourhoods in inner city Bradford, England. These neighbourhoods contain a socially and ethnically diverse population with 84% living in the poorest decile for England and Wales. Parents with a child aged 1–3 years old who are enrolled in Born in Bradford’s Better Start interventional family cohort study are eligible for this study. Intervention participants will be matched to a demographically comparable control group using propensity score matching. This study will use retrospective and prospective data from participants who attended Incredible Years groups between September 2018 and April 2024. The required minimum sample is n = 1336 (ratio 1:3) to detect a small effect (odds = 1.5, d = .20) on the Early Years Foundation Stage profile total score at age 5; a measure of early child development that is routinely collected by teachers. We will also establish whether these effects are moderated by child age at entry to intervention, programme delivery mode, socioeconomic status, and ethnicity. We will also estimate the cost of the intervention and conduct a cost-consequence analysis. (PsycInfo Database Record (c) 2024 APA, all rights reserved)</t>
+          <t>Child behavioural and mental health problems have become a public health crisis. The consequences of poor mental health in childhood have large economic costs and consequences for the individual, their families, and for society. Early intervention through parenting programmes can reduce the onset of poor mental health in childhood, hence evaluating the effectiveness of parenting programmes is critical. The 'Incredible Years Toddler' parent programme is an education and training intervention designed to enhance the social and emotional wellbeing of children aged 1-3 years. Whilst previous studies show Incredible Years Toddler to provide promising effects on child outcomes in the short term, the research samples have lacked ethnic diversity and representation from socioeconomically deprived families. This quasi-experimental study is registered on ISRCTN (ISRCTN49991769). We will investigate the effectiveness of Incredible Years Toddler being delivered in three neighbourhoods in inner city Bradford, England. These neighbourhoods contain a socially and ethnically diverse population with 84% living in the poorest decile for England and Wales. Parents with a child aged 1-3 years old who are enrolled in Born in Bradford's Better Start interventional family cohort study are eligible for this study. Intervention participants will be matched to a demographically comparable control group using propensity score matching. This study will use retrospective and prospective data from participants who attended Incredible Years groups between September 2018 and April 2024. The required minimum sample is n = 1336 (ratio 1:3) to detect a small effect (odds = 1.5, d = .20) on the Early Years Foundation Stage profile total score at age 5; a measure of early child development that is routinely collected by teachers. We will also establish whether these effects are moderated by child age at entry to intervention, programme delivery mode, socioeconomic status, and ethnicity. We will also estimate the cost of the intervention and conduct a cost-consequence analysis. (PsycInfo Database Record (c) 2024 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -2187,12 +2187,12 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>correction to: association of maternal prenatal depression and anxiety with toddler sleep: the china‑anhui birth cohort study;2022;ma</t>
+          <t>correctionto:associationofmaternalprenataldepressionandanxietywithtoddlersleep:thechina-anhuibirthcohortstudy;2022;ma</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>correction to: association of maternal prenatal depression and anxiety with toddler sleep: the china‑anhui birth cohort study</t>
+          <t>correction to: association of maternal prenatal depression and anxiety with toddler sleep: the china-anhui birth cohort study</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -2205,7 +2205,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Reports an error in 'Association of maternal prenatal depression and anxiety with toddler sleep: The China-Anhui birth cohort study' by Shuangshuang Ma, Xiaoguang Yin, Ruixue Tao, Xiaomin Jiang, Jun Xie, Pei Li, Daomin Zhu and Peng Zhu (Archives of Women's Mental Health, Advanced Online Publication, Jan 8, 2022, np). The co-first author was not noted in the original manuscript. The author Shuangshuang Ma and Xiaoguang Yin contributed equally to this study, which should be marked by a special character, and stated in the manuscript. Additionally, the authors Peng Zhu and Daomin Zhu were the corresponding authors. Their equal contribution has been noted in the online manuscript, which should remain unchanged. (The following abstract of the original article appeared in record [rid]2022-22258-001[/rid]). Maternal prenatal depression is associated with child sleep. We investigated whether maternal depression comorbid with anxiety worsens toddler’s sleep problems in a prospective cohort study. A total of 1583 mother-infant pairs from the China-Anhui Birth Cohort study were examined. The participants completed the Center for Epidemiologic Studies Depression Scale (CES-D) and Self-Rating Anxiety Scale (SAS) at 30–34 weeks of gestation, and the Edinburgh Postnatal Depression Scale (EPDS) at 3-month postpartum. Toddler’s sleep was assessed by the Brief Infant Sleep Questionnaire (BISQ) at 30 months old. Logistic regression models were used to investigate the associations between prenatal depression and anxiety and toddler’s sleep, while adjusting for maternal gestational age, education, family income, alcohol use, premature birth, fetal growth restriction, mode of delivery, postnatal depression, and 3-month breastfeeding. In total, 9.0% of participants reported prenatal depression comorbid with anxiety symptoms, and the prevalence of depression, anxiety was 6.7% and 7.3%, respectively. Compared with mothers without depression and anxiety, maternal depression combined with anxiety were significantly associated with shorter total sleep duration (11.16 ± 1.06 h), longer settling time (29.25 ± 23.57 min), and higher risk of toddlers’ sleep problems assessed by BISQ (OR = 2.09, 95% CI: 1.22–3.57) or parental report (OR = 1.84, 95% CI: 1.22–2.77). However, there was no significant association between maternal postnatal depression and toddler sleep behaviors. Maternal prenatal depression comorbid with anxiety significantly associated with poorer toddler’s sleep. Strategies to regulate prenatal mood status should be considered during prenatal health care to improve children’s sleep development. (PsycInfo Database Record (c) 2023 APA, all rights reserved)</t>
+          <t>Reports an error in 'Association of maternal prenatal depression and anxiety with toddler sleep: The China-Anhui birth cohort study' by Shuangshuang Ma, Xiaoguang Yin, Ruixue Tao, Xiaomin Jiang, Jun Xie, Pei Li, Daomin Zhu and Peng Zhu (Archives of Women's Mental Health, Advanced Online Publication, Jan 8, 2022, np). The co-first author was not noted in the original manuscript. The author Shuangshuang Ma and Xiaoguang Yin contributed equally to this study, which should be marked by a special character, and stated in the manuscript. Additionally, the authors Peng Zhu and Daomin Zhu were the corresponding authors. Their equal contribution has been noted in the online manuscript, which should remain unchanged. (The following abstract of the original article appeared in record [rid]2022-22258-001[/rid]). Maternal prenatal depression is associated with child sleep. We investigated whether maternal depression comorbid with anxiety worsens toddler's sleep problems in a prospective cohort study. A total of 1583 mother-infant pairs from the China-Anhui Birth Cohort study were examined. The participants completed the Center for Epidemiologic Studies Depression Scale (CES-D) and Self-Rating Anxiety Scale (SAS) at 30-34 weeks of gestation, and the Edinburgh Postnatal Depression Scale (EPDS) at 3-month postpartum. Toddler's sleep was assessed by the Brief Infant Sleep Questionnaire (BISQ) at 30 months old. Logistic regression models were used to investigate the associations between prenatal depression and anxiety and toddler's sleep, while adjusting for maternal gestational age, education, family income, alcohol use, premature birth, fetal growth restriction, mode of delivery, postnatal depression, and 3-month breastfeeding. In total, 9.0% of participants reported prenatal depression comorbid with anxiety symptoms, and the prevalence of depression, anxiety was 6.7% and 7.3%, respectively. Compared with mothers without depression and anxiety, maternal depression combined with anxiety were significantly associated with shorter total sleep duration (11.16 +- 1.06 h), longer settling time (29.25 +- 23.57 min), and higher risk of toddlers' sleep problems assessed by BISQ (OR = 2.09, 95% CI: 1.22-3.57) or parental report (OR = 1.84, 95% CI: 1.22-2.77). However, there was no significant association between maternal postnatal depression and toddler sleep behaviors. Maternal prenatal depression comorbid with anxiety significantly associated with poorer toddler's sleep. Strategies to regulate prenatal mood status should be considered during prenatal health care to improve children's sleep development. (PsycInfo Database Record (c) 2023 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2245,7 +2245,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>correction to: perinatal health in amazon triple border region: cross-sectional analysis comparing outcomes in the brazilian, peruvian and colombian population;2023;teixeira</t>
+          <t>correctionto:perinatalhealthinamazontripleborderregion:cross-sectionalanalysiscomparingoutcomesinthebrazilian,peruvianandcolombianpopulation;2023;teixeira</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2258,12 +2258,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Teixeira, Camila, Soares;Fernandes, Tiótrefis, Gomes;Dias, Marcos Augusto, Bastos;Morais das Neves, Milene da, Silva;Schweickardt, Julio, César;Harris, Matthew, J.;Lima, Rodrigo Tobias de, Sousa</t>
+          <t>Teixeira, Camila, Soares;Fernandes, Tiotrefis, Gomes;Dias, Marcos Augusto, Bastos;Morais das Neves, Milene da, Silva;Schweickardt, Julio, Cesar;Harris, Matthew, J.;Lima, Rodrigo Tobias de, Sousa</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Reports an error in 'Perinatal health in Amazon triple border region: Cross-sectional analysis comparing outcomes in the Brazilian, Peruvian and Colombian population' by Camila Soares Teixeira, Tiótrefis Gomes Fernandes, Marcos Augusto Bastos Dias, Milene da Silva Morais das Neves, Julio César Schweickardt, Matthew J. Harris and Rodrigo Tobias de Sousa Lima (Maternal and Child Health Journal, 2023[Oct], Vol 27[10], 1876-1884). In the original article, there were some errors in the Acknowledgements section and copyright holder name. The corrections are given in the erratum. (The following abstract of the original article appeared in record [rid]2023-80695-001[/rid]). Objective: To investigate the perinatal outcomes in Brazilian, Peruvian, and Colombian women in a Brazilian reference maternity hospital based at Amazon triple border region. Method: A cross-sectional case study of data from 3242 live birth certificates issued at the Tabatinga public maternity hospital, in the countryside of Amazonas, in the period between January 2015 and December 2017. Maternal and perinatal independent variables were analysed based on central tendency and variability, and frequency distribution for categorical variables. The Pearson’s Chi-Square test and univariate analyses were performed to estimate probability ratios (Odds Ratio-OR). Results: Significant differences were found in the education level in the three population groups, as well as in the number of previous pregnancies, antenatal consultations, month of initial prenatal care, and type of delivery. Brazilian pregnant women had more prenatal consultations, caesarean sections, and premature births. Peruvian and Colombian women started antenatal care later, and those with high-risk pregnancies tended to deliver in their home country. Conclusion for Practice: Our findings show some singularities in the care of women and infants in the Amazonian triple border region. The Brazilian Unified Health Care System performs an important role in the guarantee of free access to health services, and ensures comprehensive care for women and infants, promoting human rights in border regions regardless of nationality. Significance The triple frontier between Brazil, Colombia, and Peru is a region that has specificities that defy assistance flows, normally based on predominantly urban and locally fixed populations. Analysis of the live birth certificate data completed after the births that took place in the only public maternity hospital in this region could help to quantify and understand the migratory phenomenon and its repercussions on the health of women and their infants. Studies show that maternal and child mortality indicators are sensitive to health conditions and can reveal various aspects of a territory, such as social inequalities, socioeconomic development, and quality of life. (PsycInfo Database Record (c) 2023 APA, all rights reserved)</t>
+          <t>Reports an error in 'Perinatal health in Amazon triple border region: Cross-sectional analysis comparing outcomes in the Brazilian, Peruvian and Colombian population' by Camila Soares Teixeira, Tiotrefis Gomes Fernandes, Marcos Augusto Bastos Dias, Milene da Silva Morais das Neves, Julio Cesar Schweickardt, Matthew J. Harris and Rodrigo Tobias de Sousa Lima (Maternal and Child Health Journal, 2023[Oct], Vol 27[10], 1876-1884). In the original article, there were some errors in the Acknowledgements section and copyright holder name. The corrections are given in the erratum. (The following abstract of the original article appeared in record [rid]2023-80695-001[/rid]). Objective: To investigate the perinatal outcomes in Brazilian, Peruvian, and Colombian women in a Brazilian reference maternity hospital based at Amazon triple border region. Method: A cross-sectional case study of data from 3242 live birth certificates issued at the Tabatinga public maternity hospital, in the countryside of Amazonas, in the period between January 2015 and December 2017. Maternal and perinatal independent variables were analysed based on central tendency and variability, and frequency distribution for categorical variables. The Pearson's Chi-Square test and univariate analyses were performed to estimate probability ratios (Odds Ratio-OR). Results: Significant differences were found in the education level in the three population groups, as well as in the number of previous pregnancies, antenatal consultations, month of initial prenatal care, and type of delivery. Brazilian pregnant women had more prenatal consultations, caesarean sections, and premature births. Peruvian and Colombian women started antenatal care later, and those with high-risk pregnancies tended to deliver in their home country. Conclusion for Practice: Our findings show some singularities in the care of women and infants in the Amazonian triple border region. The Brazilian Unified Health Care System performs an important role in the guarantee of free access to health services, and ensures comprehensive care for women and infants, promoting human rights in border regions regardless of nationality. Significance The triple frontier between Brazil, Colombia, and Peru is a region that has specificities that defy assistance flows, normally based on predominantly urban and locally fixed populations. Analysis of the live birth certificate data completed after the births that took place in the only public maternity hospital in this region could help to quantify and understand the migratory phenomenon and its repercussions on the health of women and their infants. Studies show that maternal and child mortality indicators are sensitive to health conditions and can reveal various aspects of a territory, such as social inequalities, socioeconomic development, and quality of life. (PsycInfo Database Record (c) 2023 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2303,7 +2303,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>'association of maternal eating disorders with pregnancy and neonatal outcomes': correction;2020;mantel</t>
+          <t>'associationofmaternaleatingdisorderswithpregnancyandneonataloutcomes':correction;2020;mantel</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2316,12 +2316,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Mantel, Ängla;Hirschberg, Angelica, Lindén;Stephansson, Olof</t>
+          <t>Mantel, Angla;Hirschberg, Angelica, Linden;Stephansson, Olof</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Reports an error in 'Association of maternal eating disorders with pregnancy and neonatal outcomes' by Ängla Mantel, Angelica Lindén Hirschberg and Olof Stephansson (JAMA Psychiatry, 2020[Mar], Vol 77[3], 285-293). In the original article, surname of the second author was inaccurate. Angelica Lindén Hirschberg should be referred to as Dr Hirschberg, not Dr Lindén Hirschberg. The error has been corrected. (The following abstract of the original article appeared in record [rid]2020-21761-006[/rid]). Importance: The prevalence of eating disorders is high among women of reproductive age, yet the association of eating disorders with pregnancy complications and neonatal health has not been investigated in detail, to our knowledge. Objective: To investigate the relative risk of adverse pregnancy and neonatal outcomes for women with eating disorders. Design, Setting, and Participants: This population-based cohort study included all singleton births included in the Swedish Medical Birth Register from January 1, 2003, to December 31, 2014. A total of 7542 women with eating disorders were compared with 1 225 321 women without eating disorders. Statistical analysis was performed from January 1, 2018, to April 30, 2019. Via linkage with the national patient register, women with eating disorders were identified and compared with women free of any eating disorder. Eating disorders were further stratified into active or previous disease based on last time of diagnosis. Main Outcomes and Measures: The risk of adverse pregnancy outcomes (hyperemesis, anemia, preeclampsia, and antepartum hemorrhage), the mode of delivery (cesarean delivery, vaginal delivery, or instrumental vaginal delivery), and the neonatal outcomes (preterm birth, small and large sizes for gestational age, Apgar score &lt;7 at 5 minutes, and microcephaly) were calculated using Poisson regression analysis to estimate risk ratios (RRs). Models were adjusted for age, parity, smoking status, and birth year. Results: There were 2769 women with anorexia nervosa (mean [SD] age, 29.4 [5.3] years), 1378 women with bulimia nervosa (mean [SD] age, 30.2 [4.9] years), and 3395 women with an eating disorder not otherwise specified (EDNOS; mean [SD] age, 28.9 [5.3] years), and they were analyzed and compared with 1 225 321 women without eating disorders (mean [SD] age, 30.3 [5.2] years). All subtypes of maternal eating disorders were associated with an approximately 2-fold increased risk of hyperemesis during pregnancy (anorexia nervosa: RR, 2.1 [95%CI, 1.8-2.5]; bulimia nervosa: RR, 2.1 [95%CI, 1.6-2.7]; EDNOS: RR, 2.6 [95%CI, 2.3-3.0]). The risk of anemia during pregnancy was doubled for women with active anorexia nervosa (RR, 2.1 [95%CI, 1.3-3.2]) or EDNOS (RR, 2.1 [95%CI, 1.5-2.8]). Maternal anorexia nervosa was associated with an increased risk of antepartum hemorrhage (RR, 1.6 [95%CI, 1.2-2.1]), which was more pronounced in active vs previous disease.Women with anorexia nervosa (RR, 0.7 [95%CI, 0.6-0.9]) and women with EDNOS (RR, 0.8 [95%CI, 0.7-1.0]) were at decreased risk of instrumental-assisted vaginal births; otherwise, there were no major differences in mode of delivery.Women with eating disorders, all subtypes, were at increased risk of a preterm birth (anorexia nervosa: RR, 1.6 [95%CI, 1.4-1.8]; bulimia nervosa: RR, 1.3 [95%CI, 1.0-1.6]; and EDNOS: RR, 1.4 [95%CI, 1.2-1.6]) and of delivering neonates with microcephaly (anorexia nervosa: RR, 1.9 [95%CI, 1.5-2.4]; bulimia nervosa: RR, 1.6 [95%CI, 1.1-2.4]; EDNOS: RR, 1.4 [95%CI, 1.2-1.9]). Conclusions and Relevance: The findings of this study suggest that women with active or previous eating disorders, regardless of subtype, are at increased risk of adverse pregnancy and neonatal outcomes and may need increased surveillance in antenatal and delivery care. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
+          <t>Reports an error in 'Association of maternal eating disorders with pregnancy and neonatal outcomes' by Angla Mantel, Angelica Linden Hirschberg and Olof Stephansson (JAMA Psychiatry, 2020[Mar], Vol 77[3], 285-293). In the original article, surname of the second author was inaccurate. Angelica Linden Hirschberg should be referred to as Dr Hirschberg, not Dr Linden Hirschberg. The error has been corrected. (The following abstract of the original article appeared in record [rid]2020-21761-006[/rid]). Importance: The prevalence of eating disorders is high among women of reproductive age, yet the association of eating disorders with pregnancy complications and neonatal health has not been investigated in detail, to our knowledge. Objective: To investigate the relative risk of adverse pregnancy and neonatal outcomes for women with eating disorders. Design, Setting, and Participants: This population-based cohort study included all singleton births included in the Swedish Medical Birth Register from January 1, 2003, to December 31, 2014. A total of 7542 women with eating disorders were compared with 1 225 321 women without eating disorders. Statistical analysis was performed from January 1, 2018, to April 30, 2019. Via linkage with the national patient register, women with eating disorders were identified and compared with women free of any eating disorder. Eating disorders were further stratified into active or previous disease based on last time of diagnosis. Main Outcomes and Measures: The risk of adverse pregnancy outcomes (hyperemesis, anemia, preeclampsia, and antepartum hemorrhage), the mode of delivery (cesarean delivery, vaginal delivery, or instrumental vaginal delivery), and the neonatal outcomes (preterm birth, small and large sizes for gestational age, Apgar score &lt;7 at 5 minutes, and microcephaly) were calculated using Poisson regression analysis to estimate risk ratios (RRs). Models were adjusted for age, parity, smoking status, and birth year. Results: There were 2769 women with anorexia nervosa (mean [SD] age, 29.4 [5.3] years), 1378 women with bulimia nervosa (mean [SD] age, 30.2 [4.9] years), and 3395 women with an eating disorder not otherwise specified (EDNOS; mean [SD] age, 28.9 [5.3] years), and they were analyzed and compared with 1 225 321 women without eating disorders (mean [SD] age, 30.3 [5.2] years). All subtypes of maternal eating disorders were associated with an approximately 2-fold increased risk of hyperemesis during pregnancy (anorexia nervosa: RR, 2.1 [95%CI, 1.8-2.5]; bulimia nervosa: RR, 2.1 [95%CI, 1.6-2.7]; EDNOS: RR, 2.6 [95%CI, 2.3-3.0]). The risk of anemia during pregnancy was doubled for women with active anorexia nervosa (RR, 2.1 [95%CI, 1.3-3.2]) or EDNOS (RR, 2.1 [95%CI, 1.5-2.8]). Maternal anorexia nervosa was associated with an increased risk of antepartum hemorrhage (RR, 1.6 [95%CI, 1.2-2.1]), which was more pronounced in active vs previous disease.Women with anorexia nervosa (RR, 0.7 [95%CI, 0.6-0.9]) and women with EDNOS (RR, 0.8 [95%CI, 0.7-1.0]) were at decreased risk of instrumental-assisted vaginal births; otherwise, there were no major differences in mode of delivery.Women with eating disorders, all subtypes, were at increased risk of a preterm birth (anorexia nervosa: RR, 1.6 [95%CI, 1.4-1.8]; bulimia nervosa: RR, 1.3 [95%CI, 1.0-1.6]; and EDNOS: RR, 1.4 [95%CI, 1.2-1.6]) and of delivering neonates with microcephaly (anorexia nervosa: RR, 1.9 [95%CI, 1.5-2.4]; bulimia nervosa: RR, 1.6 [95%CI, 1.1-2.4]; EDNOS: RR, 1.4 [95%CI, 1.2-1.9]). Conclusions and Relevance: The findings of this study suggest that women with active or previous eating disorders, regardless of subtype, are at increased risk of adverse pregnancy and neonatal outcomes and may need increased surveillance in antenatal and delivery care. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -2359,7 +2359,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>cesarean delivery under general anesthesia causing autistic spectrum disorders: not very likely;2020;raz</t>
+          <t>cesareandeliveryundergeneralanesthesiacausingautisticspectrumdisorders:notverylikely;2020;raz</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Comments on an article by S. M. Huberman et al. (see record [rid]2019-25374-001[/rid]). The authors performed a case–control study using analysis of patient charts with the intention to characterize the role of labor and delivery in the development of autistic spectrum disorders. They found a statistical correlation between cesarean delivery conducted under general anesthesia and later development of autism. The commenting authors note that the study design may lead to false conclusions, based on how the groups are selected. Thus, the results cannot support the conclusion of a causal relation. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
+          <t>Comments on an article by S. M. Huberman et al. (see record [rid]2019-25374-001[/rid]). The authors performed a case-control study using analysis of patient charts with the intention to characterize the role of labor and delivery in the development of autistic spectrum disorders. They found a statistical correlation between cesarean delivery conducted under general anesthesia and later development of autism. The commenting authors note that the study design may lead to false conclusions, based on how the groups are selected. Thus, the results cannot support the conclusion of a causal relation. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2417,7 +2417,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>correction to: predicting risk for early breastfeeding cessation in israel;2022;gabay</t>
+          <t>correctionto:predictingriskforearlybreastfeedingcessationinisrael;2022;gabay</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Reports an error in 'Predicting risk for early breastfeeding cessation in Israel' by Zarina Paltiel Gabay, Kaboni Whitney Gondwe and Maxim Topaz (Maternal and Child Health Journal, Advanced Online Publication, Dec 2, 2021, np). The original version of this article contained a mistake. In the methods section, under sub-heading 'Study Design'—the text 'XXXX' should be replaced with the university name. The correct sentence is given in the erratum. (The following abstract of the original article appeared in record [rid]2022-11994-001[/rid]). Objectives: This study aimed to 1) Examine factors associated with cessation of exclusive breastfeeding in Israel and 2) Develop predictive models to identify women at risk for early exclusive breastfeeding cessation. Methods: The study used data from longitudinal national representative infant nutrition survey in Israel (n = 2119 participants). Logistic regression was used to identify risk factors and build predictive models. Results: The rate of exclusive breastfeeding cessation increased from 45.4% at 2 months to 85.7% at 6 months. Five factors were significantly associated with higher odds of exclusive breastfeeding cessation at 2 months: being a primapara, low educational level, lack of previous breastfeeding experience, negative attitude towards birth, and lack of intention to breastfeed. Six factors were significantly associated with higher odds of exclusive breastfeeding cessation at 6 months: younger age, being in a relationship with a partner, lower religiosity level, cesarean delivery, not taking folic acid during pregnancy, and negative attitude towards birth. Both 2 and 6-months models had good predictive performance (C-statistic of .72 and .68, accordingly). Conclusions for Practice: This nationwide study successfully identified several predictors of exclusive breastfeeding cessation and created breastfeeding cessation prediction tools for two time periods (2 and 6 months). The resulting tools can be applied to identify women at risk for stopping exclusive breastfeeding in hospitals or at community clinics. Further studies should examine practical aspects of applying these tools in practice and explore whether applying those tools can lead to higher exclusive breastfeeding rates. (PsycInfo Database Record (c) 2023 APA, all rights reserved)</t>
+          <t>Reports an error in 'Predicting risk for early breastfeeding cessation in Israel' by Zarina Paltiel Gabay, Kaboni Whitney Gondwe and Maxim Topaz (Maternal and Child Health Journal, Advanced Online Publication, Dec 2, 2021, np). The original version of this article contained a mistake. In the methods section, under sub-heading 'Study Design'--the text 'XXXX' should be replaced with the university name. The correct sentence is given in the erratum. (The following abstract of the original article appeared in record [rid]2022-11994-001[/rid]). Objectives: This study aimed to 1) Examine factors associated with cessation of exclusive breastfeeding in Israel and 2) Develop predictive models to identify women at risk for early exclusive breastfeeding cessation. Methods: The study used data from longitudinal national representative infant nutrition survey in Israel (n = 2119 participants). Logistic regression was used to identify risk factors and build predictive models. Results: The rate of exclusive breastfeeding cessation increased from 45.4% at 2 months to 85.7% at 6 months. Five factors were significantly associated with higher odds of exclusive breastfeeding cessation at 2 months: being a primapara, low educational level, lack of previous breastfeeding experience, negative attitude towards birth, and lack of intention to breastfeed. Six factors were significantly associated with higher odds of exclusive breastfeeding cessation at 6 months: younger age, being in a relationship with a partner, lower religiosity level, cesarean delivery, not taking folic acid during pregnancy, and negative attitude towards birth. Both 2 and 6-months models had good predictive performance (C-statistic of .72 and .68, accordingly). Conclusions for Practice: This nationwide study successfully identified several predictors of exclusive breastfeeding cessation and created breastfeeding cessation prediction tools for two time periods (2 and 6 months). The resulting tools can be applied to identify women at risk for stopping exclusive breastfeeding in hospitals or at community clinics. Further studies should examine practical aspects of applying these tools in practice and explore whether applying those tools can lead to higher exclusive breastfeeding rates. (PsycInfo Database Record (c) 2023 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -2473,12 +2473,12 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>'changes in rates of inpatient postpartum long-acting reversible contraception and sterilization in the usa, 2012–2016': correction;2021;sheyn</t>
+          <t>'changesinratesofinpatientpostpartumlong-actingreversiblecontraceptionandsterilizationintheusa,2012-2016':correction;2021;sheyn</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>'changes in rates of inpatient postpartum long-acting reversible contraception and sterilization in the usa, 2012–2016': correction</t>
+          <t>'changes in rates of inpatient postpartum long-acting reversible contraception and sterilization in the usa, 2012-2016': correction</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Reports an error in 'Changes in rates of inpatient postpartum long-acting reversible contraception and sterilization in the USA, 2012–2016' by David Sheyn and Kavita Shah Arora (Maternal and Child Health Journal, Advanced Online Publication, May 10, 2021, np). In the original article, there was a mistake in the supplementary file. The delivery DRG codes were incorrect in Supplementary Table 1. The Supplementary Table 1 is corrected. (The following abstract of the original article appeared in record [rid]2021-45309-001[/rid]). Objectives To examine recent rates of long-acting and permanent methods (LAPM) of contraception use during delivery hospitalization and correlates of their use. Methods A retrospective cohort study utilizing the 2012–2016 National Inpatient Sample of hospitalizations in the United States of America. The International Classification of Diseases, 9th and 10th Revision, Clinical Modification codes were used to identify deliveries, inpatient long-acting reversible contraception (IPP LARC), and postpartum tubal ligation (PPTL). We conducted univariable and multivariable logistic regression to examine associations between demographic, clinical, hospital and geographical characteristics with likelihood of LAPM including IPP LARC and PPTL. Results Our sample included 3,642,328 unweighted deliveries. The rate of IPP LARC increased from 34.6 to 54.9 per 10,000 deliveries (58.7%), while the rate of PPTL utilization decreased from 719.5 to 671.8 per 10,000 deliveries (6.6%) over the study period. In multivariable analysis of LAPM utilization versus neither, cesarean delivery (aOR 7.25, 95% CI 7.08–7.43) was associated with greater utilization. Native American (aOR 4.01, 95% CI 2.91–5.53) race was associated with increased use of IPP LARC compared to a non-long-acting method of contraception. Age between 18 and 29 years (aOR 6.21, 95% CI 5.42–7.11) was associated with greater use of IPP LARC versus PPTL. Delivering in a rural hospital ((aOR 0.09, 95% CI 0.06–0.12) and cesarean delivery (aOR 0.09, 95% CI 0.06–0.12) were associated with greater use PPTL versus IPP LARC. Conclusions The IPP LARC rate remains at less than 10% the PPTL rates in our study timeframe. The demonstrated variation in uptake of highly effective methods of contraception inpatient after delivery offer possible opportunities for better understanding and improvement in access. (PsycInfo Database Record (c) 2021 APA, all rights reserved)</t>
+          <t>Reports an error in 'Changes in rates of inpatient postpartum long-acting reversible contraception and sterilization in the USA, 2012-2016' by David Sheyn and Kavita Shah Arora (Maternal and Child Health Journal, Advanced Online Publication, May 10, 2021, np). In the original article, there was a mistake in the supplementary file. The delivery DRG codes were incorrect in Supplementary Table 1. The Supplementary Table 1 is corrected. (The following abstract of the original article appeared in record [rid]2021-45309-001[/rid]). Objectives To examine recent rates of long-acting and permanent methods (LAPM) of contraception use during delivery hospitalization and correlates of their use. Methods A retrospective cohort study utilizing the 2012-2016 National Inpatient Sample of hospitalizations in the United States of America. The International Classification of Diseases, 9th and 10th Revision, Clinical Modification codes were used to identify deliveries, inpatient long-acting reversible contraception (IPP LARC), and postpartum tubal ligation (PPTL). We conducted univariable and multivariable logistic regression to examine associations between demographic, clinical, hospital and geographical characteristics with likelihood of LAPM including IPP LARC and PPTL. Results Our sample included 3,642,328 unweighted deliveries. The rate of IPP LARC increased from 34.6 to 54.9 per 10,000 deliveries (58.7%), while the rate of PPTL utilization decreased from 719.5 to 671.8 per 10,000 deliveries (6.6%) over the study period. In multivariable analysis of LAPM utilization versus neither, cesarean delivery (aOR 7.25, 95% CI 7.08-7.43) was associated with greater utilization. Native American (aOR 4.01, 95% CI 2.91-5.53) race was associated with increased use of IPP LARC compared to a non-long-acting method of contraception. Age between 18 and 29 years (aOR 6.21, 95% CI 5.42-7.11) was associated with greater use of IPP LARC versus PPTL. Delivering in a rural hospital ((aOR 0.09, 95% CI 0.06-0.12) and cesarean delivery (aOR 0.09, 95% CI 0.06-0.12) were associated with greater use PPTL versus IPP LARC. Conclusions The IPP LARC rate remains at less than 10% the PPTL rates in our study timeframe. The demonstrated variation in uptake of highly effective methods of contraception inpatient after delivery offer possible opportunities for better understanding and improvement in access. (PsycInfo Database Record (c) 2021 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -2531,12 +2531,12 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>long-term survival in a patient with muscle–eye–brain disease;2015;falsaperla</t>
+          <t>long-termsurvivalinapatientwithmuscle-eye-braindisease;2015;falsaperla</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>long-term survival in a patient with muscle–eye–brain disease</t>
+          <t>long-term survival in a patient with muscle-eye-brain disease</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Presents a case report of a 13 year old girl. V.E. was born at 37 weeks of gestation by caesarian section for membranes' premature rupture. Her weight at birth was 2850 g, height 48 cm, and Head Circumference (HC) 34 cm. Her familial anamnesis was negative for neuromuscular disorders and any other neurologic disorders. The peculiar findings of author's case are that the patient they described had a less severe course than other cases of muscle–eye–brain disease (MEB) since now reported in the literature, with unusual brain- MRI features for the disease, showing cortical gyration anomalies and cortical cerebellum multicystic degeneration, to their knowledge, never previously described in the literature. Recently a survey on clinical, radiological and genetic features of patients with MEB disease, caused by POMGNT1 mutation, has been published and from a cohort of 34 patients with CMD, 12 patients from 10 families were diagnosed with MEB disease. In these patients, authors found that the most common radiologic abnormalities were periventricular white matter abnormalities, ventriculomegaly, pontocerebellar hypoplasia, and multiple cerebellar cysts. All of the patients had mutations in the POMGNT1 gene. Author's concluded that MEB is caused by different mutations of POMGNT1 gene, some of which show a milder course, with peculiar clinical and radiological findings. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
+          <t>Presents a case report of a 13 year old girl. V.E. was born at 37 weeks of gestation by caesarian section for membranes' premature rupture. Her weight at birth was 2850 g, height 48 cm, and Head Circumference (HC) 34 cm. Her familial anamnesis was negative for neuromuscular disorders and any other neurologic disorders. The peculiar findings of author's case are that the patient they described had a less severe course than other cases of muscle-eye-brain disease (MEB) since now reported in the literature, with unusual brain- MRI features for the disease, showing cortical gyration anomalies and cortical cerebellum multicystic degeneration, to their knowledge, never previously described in the literature. Recently a survey on clinical, radiological and genetic features of patients with MEB disease, caused by POMGNT1 mutation, has been published and from a cohort of 34 patients with CMD, 12 patients from 10 families were diagnosed with MEB disease. In these patients, authors found that the most common radiologic abnormalities were periventricular white matter abnormalities, ventriculomegaly, pontocerebellar hypoplasia, and multiple cerebellar cysts. All of the patients had mutations in the POMGNT1 gene. Author's concluded that MEB is caused by different mutations of POMGNT1 gene, some of which show a milder course, with peculiar clinical and radiological findings. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2589,7 +2589,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>why not induce everyone at 39 weeks?;2017;glantz</t>
+          <t>whynotinduceeveryoneat39weeks?;2017;glantz</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2647,7 +2647,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>risks during pregnancy in women with epilepsy;2015;meador</t>
+          <t>risksduringpregnancyinwomenwithepilepsy;2015;meador</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Comments on an article by Luz Viale et al. (see record [rid]2015-51800-036[/rid]). Viale et al. present the results of their systematic review and metaanalysis of observational studies to assess risks of maternal and fetal complications (excluding malformations and cognitive-behavioral deficits). Viale et al. analyses included 38 studies with 2837325 pregnancies. Women with epilepsy versus those without epilepsy had increased risks for spontaneous miscarriage (odds ratio [OR] 1·54, 95% CI 1·02–2·32), antepartum hemorrhage (1·49, 1·01–2·20), postpartum hemorrhage (1·29, 1·13–1·49), hypertensive disorders (1·37, 1·21–1·55), induction of labor (1·67, 1·31–2·11), caesarean section (1·40, 1·23–1·58), any preterm birth (1·16, 1·01–1·34), and fetal growth restriction (1·26, 1·20–1·33). Viale et al. conclude that epilepsy and exposure to antiepileptic drugs are associated with a small but significant risk for several adverse outcomes during pregnancy. Viale et al. study is well conducted and adds to existing published work by providing improved estimates for several risks during pregnancy in women with epilepsy. (PsycINFO Database Record (c) 2016 APA, all rights reserved)</t>
+          <t>Comments on an article by Luz Viale et al. (see record [rid]2015-51800-036[/rid]). Viale et al. present the results of their systematic review and metaanalysis of observational studies to assess risks of maternal and fetal complications (excluding malformations and cognitive-behavioral deficits). Viale et al. analyses included 38 studies with 2837325 pregnancies. Women with epilepsy versus those without epilepsy had increased risks for spontaneous miscarriage (odds ratio [OR] 1*54, 95% CI 1*02-2*32), antepartum hemorrhage (1*49, 1*01-2*20), postpartum hemorrhage (1*29, 1*13-1*49), hypertensive disorders (1*37, 1*21-1*55), induction of labor (1*67, 1*31-2*11), caesarean section (1*40, 1*23-1*58), any preterm birth (1*16, 1*01-1*34), and fetal growth restriction (1*26, 1*20-1*33). Viale et al. conclude that epilepsy and exposure to antiepileptic drugs are associated with a small but significant risk for several adverse outcomes during pregnancy. Viale et al. study is well conducted and adds to existing published work by providing improved estimates for several risks during pregnancy in women with epilepsy. (PsycINFO Database Record (c) 2016 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -2705,7 +2705,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>tokophobia, the fear of childbirth, and the decision to breastfeed;2015;kaymaz</t>
+          <t>tokophobia,thefearofchildbirth,andthedecisiontobreastfeed;2015;kaymaz</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2718,7 +2718,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Kaymaz, Nazan;Uzun, Mehmet, Erdem;Yıldırım, Şule</t>
+          <t>Kaymaz, Nazan;Uzun, Mehmet, Erdem;Yildirim, Sule</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -2761,7 +2761,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>'narcolepsy and pregnancy: a retrospective european evaluation of 249 pregnancies:' corrigendum;2014;maurovich‐horvat</t>
+          <t>'narcolepsyandpregnancy:aretrospectiveeuropeanevaluationof249pregnancies:'corrigendum;2014;maurovich-horvat</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2774,12 +2774,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Maurovich‐Horvat, Eszter;Kemlink, David;Högl, Birgit;Frauscher, Birgit;Ehrmann, Laura;Geisler, Peter;Ettenhuber, Katharina;Mayer, Geert;Peraita‐Adrados, Rosa;Calvo, Elena;Lammers, Gert, Jan;van der Heide, Astrid;Ferini‐Strambi, Luigi;Plazzi, Giuseppe;Poli, Francesca;Dauvilliers, Yves;Jennum, Poul;Leonthin, Helle;Mathis, Johannes;Wierzbicka, Aleksandra;Puertas, Francisco, J.;Beitinger, Pierre, A.;Arnulf, Isabelle;Riha, Renata, L.;Tormášiová, Maria;Slonková, Jana;Nevšímalová, Sona;Šonka, Karel</t>
+          <t>Maurovich-Horvat, Eszter;Kemlink, David;Hogl, Birgit;Frauscher, Birgit;Ehrmann, Laura;Geisler, Peter;Ettenhuber, Katharina;Mayer, Geert;Peraita-Adrados, Rosa;Calvo, Elena;Lammers, Gert, Jan;van der Heide, Astrid;Ferini-Strambi, Luigi;Plazzi, Giuseppe;Poli, Francesca;Dauvilliers, Yves;Jennum, Poul;Leonthin, Helle;Mathis, Johannes;Wierzbicka, Aleksandra;Puertas, Francisco, J.;Beitinger, Pierre, A.;Arnulf, Isabelle;Riha, Renata, L.;Tormasiova, Maria;Slonkova, Jana;Nevsimalova, Sona;Sonka, Karel</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Reports an error in 'Narcolepsy and pregnancy: A retrospective European evaluation of 249 pregnancies' by Eszter Maurovich‐Horvat, David Kemlink, Birgit Högl, Birgit Frauscher, Laura Ehrmann, Peter Geisler, Katharina Ettenhuber, Geert Mayer, Rosa Peraita‐Adrados, Elena Calvo, Gert Jan Lammers, Astrid van der Heide, Luigi Ferini‐Strambi, Giuseppe Plazzi, Francesca Poli, Yves Dauvilliers, Poul Jennum, Helle Leonthin, Johannes Mathis, Aleksandra Wierzbicka, Francisco J. Puertas, Pierre A. Beitinger, Isabelle Arnulf, Renata L. Riha, Maria Tormášiová, Jana Slonková, Sona Nevšímalová and Karel Šonka (Journal of Sleep Research, 2013[Oct], Vol 22[5], 496-512). In the original article, there were two errors in the affiliations. The corrections are present in the erratum. (The following abstract of the original article appeared in record [rid]2013-33304-004[/rid]). In a retrospective cohort study undertaken in 12 European countries, 249 female narcoleptic patients with cataplexy (n = 216) and without cataplexy (n = 33) completed a self‐administrated questionnaire regarding pregnancy and childbirth. The cohort was divided further into patients whose symptoms of narcolepsy started before or during pregnancy (308 pregnancies) and those in whom the first symptoms of narcolepsy appeared after delivery (106 pregnancies). Patients with narcolepsy during pregnancy were older during their first pregnancy (P &lt; 0.001) and had a higher body mass index (BMI) prior to pregnancy (P &lt; 0.01). Weight gain during pregnancy was higher in narcoleptic patients with cataplexy (P &lt; 0.01). More patients with narcolepsy–cataplexy during pregnancy had impaired glucose metabolism and anaemia. Three patients experienced cataplexy during delivery. The rate of caesarean sections was higher in the narcolepsy–cataplexy group compared to the narcolepsy group (P &lt; 0.05). The mean birth weight and gestational age of neonates were within the normal range and did not differ across groups. Neonatal care was affected adversely by symptoms of narcolepsy in 60.1% of those with narcolepsy during pregnancy. This study reports more obstetric complications in patients with narcolepsy–cataplexy during pregnancy; however, these were not severe. This group also had a higher BMI and higher incidence of impaired glucose metabolism during pregnancy. Caesarian section was conducted more frequently in narcolepsy–cataplexy patients, despite cataplexy being a rare event during delivery. Furthermore, symptoms of narcolepsy may render care of the infant more difficult. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
+          <t>Reports an error in 'Narcolepsy and pregnancy: A retrospective European evaluation of 249 pregnancies' by Eszter Maurovich-Horvat, David Kemlink, Birgit Hogl, Birgit Frauscher, Laura Ehrmann, Peter Geisler, Katharina Ettenhuber, Geert Mayer, Rosa Peraita-Adrados, Elena Calvo, Gert Jan Lammers, Astrid van der Heide, Luigi Ferini-Strambi, Giuseppe Plazzi, Francesca Poli, Yves Dauvilliers, Poul Jennum, Helle Leonthin, Johannes Mathis, Aleksandra Wierzbicka, Francisco J. Puertas, Pierre A. Beitinger, Isabelle Arnulf, Renata L. Riha, Maria Tormasiova, Jana Slonkova, Sona Nevsimalova and Karel Sonka (Journal of Sleep Research, 2013[Oct], Vol 22[5], 496-512). In the original article, there were two errors in the affiliations. The corrections are present in the erratum. (The following abstract of the original article appeared in record [rid]2013-33304-004[/rid]). In a retrospective cohort study undertaken in 12 European countries, 249 female narcoleptic patients with cataplexy (n = 216) and without cataplexy (n = 33) completed a self-administrated questionnaire regarding pregnancy and childbirth. The cohort was divided further into patients whose symptoms of narcolepsy started before or during pregnancy (308 pregnancies) and those in whom the first symptoms of narcolepsy appeared after delivery (106 pregnancies). Patients with narcolepsy during pregnancy were older during their first pregnancy (P &lt; 0.001) and had a higher body mass index (BMI) prior to pregnancy (P &lt; 0.01). Weight gain during pregnancy was higher in narcoleptic patients with cataplexy (P &lt; 0.01). More patients with narcolepsy-cataplexy during pregnancy had impaired glucose metabolism and anaemia. Three patients experienced cataplexy during delivery. The rate of caesarean sections was higher in the narcolepsy-cataplexy group compared to the narcolepsy group (P &lt; 0.05). The mean birth weight and gestational age of neonates were within the normal range and did not differ across groups. Neonatal care was affected adversely by symptoms of narcolepsy in 60.1% of those with narcolepsy during pregnancy. This study reports more obstetric complications in patients with narcolepsy-cataplexy during pregnancy; however, these were not severe. This group also had a higher BMI and higher incidence of impaired glucose metabolism during pregnancy. Caesarian section was conducted more frequently in narcolepsy-cataplexy patients, despite cataplexy being a rare event during delivery. Furthermore, symptoms of narcolepsy may render care of the infant more difficult. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -2810,14 +2810,14 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Maurovich‐Horvat</t>
+          <t>Maurovich-Horvat</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>continuation versus discontinuation of lithium during pregnancy: a retrospective case series;2014;deiana</t>
+          <t>continuationversusdiscontinuationoflithiumduringpregnancy:aretrospectivecaseseries;2014;deiana</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2875,7 +2875,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>maternal antidepressant use and persistent pulmonary hypertension of the newborn;2015;giannakopoulos</t>
+          <t>maternalantidepressantuseandpersistentpulmonaryhypertensionofthenewborn;2015;giannakopoulos</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2933,7 +2933,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>women with epilepsy;2016;sharma</t>
+          <t>womenwithepilepsy;2016;sharma</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2946,7 +2946,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Sharma, Anumeha;Boller, François;Koubeissi, Mohamad</t>
+          <t>Sharma, Anumeha;Boller, Francois;Koubeissi, Mohamad</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -2985,7 +2985,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>'symptoms of eating disorders and feeding practices in obese mothers': corrigendum;2014;zanardo</t>
+          <t>'symptomsofeatingdisordersandfeedingpracticesinobesemothers':corrigendum;2014;zanardo</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -3003,7 +3003,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Reports an error in 'Symptoms of eating disorders and feeding practices in obese mothers' by Vincenzo Zanardo, Gianluca Straface, Barbara Benevento, Irene Gambina, Francesco Cavallin and Daniele Trevisanuto (Early Human Development, 2014[Feb], Vol 90[2], 93-96). In the original article, the affiliation of Francesco Cavallin was incorrectly given. The corrected affiliation of the author is present in the erratum. (The following abstract of the original article appeared in record [rid]2014-03695-005[/rid]). Background: The potential that obesity in pregnancy has to affect symptoms associated with eating disorders and breastfeeding is unclear. Aim: This study analyzed symptoms of eating disorders and breastfeeding practices in obese mothers. Study design: Prospective, case–control study. Subjects: Participants included 25 obese (BMI &gt; 30 kg/m²) and 25 normal-weight puerperae, matched for parity and delivery route. Outcome measures: The participants completed the Eating Disorders Inventory (EDI-2), investigating cognitive, emotional, and behavioral symptoms of eating disorders before they were discharged from the maternity hospital and later participated in telephone interviews concerning breastfeeding practices which were classified according to WHO definitions. Results: Although none of the scores fell in the pathological range, the obese mothers had more and more pronounced symptoms of eating disorders in all EDI-2 subscales with respect to normal-weight mothers. They had, in particular, significantly higher scores in body dissatisfaction (p &lt; .0001), ineffectiveness (p = .004), interoceptive awareness (p = .005), and maturity fear (p = .007). Finally, while breastfeeding practices were similar in the two groups, the obese mothers were more likely to maintain full breastfeeding at 6 months (20 vs 8%) and their tendency to postpone weaning was found to be significant (p &lt; .04). Conclusions: While the obese mothers studied have more pronounced symptoms of eating disorders with respect to their normal-weight counterparts, they tended to maintain breastfeeding longer, postponing weaning. (PsycINFO Database Record (c) 2017 APA, all rights reserved)</t>
+          <t>Reports an error in 'Symptoms of eating disorders and feeding practices in obese mothers' by Vincenzo Zanardo, Gianluca Straface, Barbara Benevento, Irene Gambina, Francesco Cavallin and Daniele Trevisanuto (Early Human Development, 2014[Feb], Vol 90[2], 93-96). In the original article, the affiliation of Francesco Cavallin was incorrectly given. The corrected affiliation of the author is present in the erratum. (The following abstract of the original article appeared in record [rid]2014-03695-005[/rid]). Background: The potential that obesity in pregnancy has to affect symptoms associated with eating disorders and breastfeeding is unclear. Aim: This study analyzed symptoms of eating disorders and breastfeeding practices in obese mothers. Study design: Prospective, case-control study. Subjects: Participants included 25 obese (BMI &gt; 30 kg/m2) and 25 normal-weight puerperae, matched for parity and delivery route. Outcome measures: The participants completed the Eating Disorders Inventory (EDI-2), investigating cognitive, emotional, and behavioral symptoms of eating disorders before they were discharged from the maternity hospital and later participated in telephone interviews concerning breastfeeding practices which were classified according to WHO definitions. Results: Although none of the scores fell in the pathological range, the obese mothers had more and more pronounced symptoms of eating disorders in all EDI-2 subscales with respect to normal-weight mothers. They had, in particular, significantly higher scores in body dissatisfaction (p &lt; .0001), ineffectiveness (p = .004), interoceptive awareness (p = .005), and maturity fear (p = .007). Finally, while breastfeeding practices were similar in the two groups, the obese mothers were more likely to maintain full breastfeeding at 6 months (20 vs 8%) and their tendency to postpone weaning was found to be significant (p &lt; .04). Conclusions: While the obese mothers studied have more pronounced symptoms of eating disorders with respect to their normal-weight counterparts, they tended to maintain breastfeeding longer, postponing weaning. (PsycINFO Database Record (c) 2017 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -3041,7 +3041,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>'maternal antidepressant use and persistent pulmonary hypertension of the newborn': in reply;2015;huybrechts</t>
+          <t>'maternalantidepressantuseandpersistentpulmonaryhypertensionofthenewborn':inreply;2015;huybrechts</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -3099,7 +3099,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>'a study of postpartum depression and maternal risk factors in qatar': corrigendum;2015;burgut</t>
+          <t>'astudyofpostpartumdepressionandmaternalriskfactorsinqatar':corrigendum;2015;burgut</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -3117,7 +3117,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Reports an error in 'A study of postpartum depression and maternal risk factors in Qatar' by F. Tuna Burgut, Abdulbari Bener, Suheila Ghuloum and Javaid Sheikh (Journal of Psychosomatic Obstetrics &amp; Gynecology, 2013[Jun], Vol 34[2], 90-97). In the original article, the authors omitted the following reference: Bener A, Burgut FT, Ghuloum S, Sheikh J. A study of postpartum depression in a fast developing country: prevalence and related factors. Int J Psychiat Med 2012;43:325–337. (The following abstract of the original article appeared in record [rid]2013-19649-006[/rid]). Objective: The objective of this study was to investigate the association between maternal complications and postpartum depression (PPD) among postpartum women in Qatar by using the Edinburgh Postnatal Depression Scale (EPDS) as well as a structured questionnaire. Methods: This is a cross-sectional study of PPD of 1379 postpartum women within 6 months of delivery attending the primary healthcare centers of the State of Qatar. Results: The prevalence of PPD was 17.6% in the studied mothers. The results of the logistic regression analysis showed that the risk factors for PPD included various socio-demographic risk factors such as education, occupation, consanguinity and access to transportation. Amongst the maternal factors studied, history of unplanned pregnancy and infertility and other medical complications such as gestational diabetes, heart disease, threatened abortion and cesarean section were found to be risk factors for PPD. Amongst the postpartum women with maternal complications, items related to feeling scared and panicky and feeling sad and miserable were the most frequently reported symptoms of depression. These women were also more likely to be experiencing sleep difficulty (p = 0.029) compared to women without maternal complications. Conclusion: While socio-demographic risk factors are well studied in the PPD literature, there is much less information on the impact of maternal complications on the psychological status of postpartum women. Postpartum women, especially those with maternal complications, need close screening and have quick access to mental healthcare within integrated reproductive health services. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
+          <t>Reports an error in 'A study of postpartum depression and maternal risk factors in Qatar' by F. Tuna Burgut, Abdulbari Bener, Suheila Ghuloum and Javaid Sheikh (Journal of Psychosomatic Obstetrics &amp; Gynecology, 2013[Jun], Vol 34[2], 90-97). In the original article, the authors omitted the following reference: Bener A, Burgut FT, Ghuloum S, Sheikh J. A study of postpartum depression in a fast developing country: prevalence and related factors. Int J Psychiat Med 2012;43:325-337. (The following abstract of the original article appeared in record [rid]2013-19649-006[/rid]). Objective: The objective of this study was to investigate the association between maternal complications and postpartum depression (PPD) among postpartum women in Qatar by using the Edinburgh Postnatal Depression Scale (EPDS) as well as a structured questionnaire. Methods: This is a cross-sectional study of PPD of 1379 postpartum women within 6 months of delivery attending the primary healthcare centers of the State of Qatar. Results: The prevalence of PPD was 17.6% in the studied mothers. The results of the logistic regression analysis showed that the risk factors for PPD included various socio-demographic risk factors such as education, occupation, consanguinity and access to transportation. Amongst the maternal factors studied, history of unplanned pregnancy and infertility and other medical complications such as gestational diabetes, heart disease, threatened abortion and cesarean section were found to be risk factors for PPD. Amongst the postpartum women with maternal complications, items related to feeling scared and panicky and feeling sad and miserable were the most frequently reported symptoms of depression. These women were also more likely to be experiencing sleep difficulty (p = 0.029) compared to women without maternal complications. Conclusion: While socio-demographic risk factors are well studied in the PPD literature, there is much less information on the impact of maternal complications on the psychological status of postpartum women. Postpartum women, especially those with maternal complications, need close screening and have quick access to mental healthcare within integrated reproductive health services. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -3562,12 +3562,12 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>prenatal psychological distress and 11β-hsd2 gene expression in human placentas: systematic review and meta-analysis;2024;tartour</t>
+          <t>prenatalpsychologicaldistressand11b-hsd2geneexpressioninhumanplacentas:systematicreviewandmeta-analysis;2024;tartour</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>prenatal psychological distress and 11β-hsd2 gene expression in human placentas: systematic review and meta-analysis</t>
+          <t>prenatal psychological distress and 11b-hsd2 gene expression in human placentas: systematic review and meta-analysis</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -3580,7 +3580,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Background: The placenta acts as a buffer to regulate the degree of fetal exposure to maternal cortisol through the 11-Beta Hydroxysteroid Dehydrogenase isoenzyme type 2 (11-β HSD2) enzyme. We conducted a systematic review and meta-analysis to assess the effect of prenatal psychological distress (PPD) on placental 11-β HSD2 gene expression and explore the related mechanistic pathways involved in fetal neurodevelopment. Methods: We searched PubMed, Embase, Scopus, APA PsycInfo®, and ProQuest Dissertations for observational studies assessing the association between PPD and 11-β HSD2 expression in human placentas. Adjusted regression coefficients (β) and corresponding 95% confidence intervals (CIs) were pooled based on three contextual PPD exposure groups: prenatal depression, anxiety symptoms, and perceived stress. Results: Of 3159 retrieved records, sixteen longitudinal studies involving 1869 participants across seven countries were included. Overall, exposure to PPD disorders showed weak negative associations with the placental 11-β HSD2 gene expression as follows: prenatal depression (β −0.01, 95% CI 0.05–0.02, I2=0%), anxiety symptoms (β −0.02, 95% CI 0.06–0.01, I2=0%), and perceived stress (β −0.01 95% CI 0.06–0.04, I2=62.8%). Third-trimester PPD exposure was more frequently associated with lower placental 11-β HSD2 levels. PPD and placental 11-β HSD2 were associated with changes in cortisol reactivity and the development of adverse health outcomes in mothers and children. Female-offspring were more vulnerable to PPD exposures. Conclusion: The study presents evidence of a modest role of prenatal psychological distress in regulating placental 11-β HSD2 gene expression. Future prospective cohorts utilizing larger sample sizes or advanced statistical methods to enhance the detection of small effect sizes should be planned. Additionally, controlling for key predictors such as the mother’s ethnicity, trimester of PPD exposure, mode of delivery, and infant sex is crucial for valid exploration of PPD effects on fetal programming. (PsycInfo Database Record (c) 2024 APA, all rights reserved)</t>
+          <t>Background: The placenta acts as a buffer to regulate the degree of fetal exposure to maternal cortisol through the 11-Beta Hydroxysteroid Dehydrogenase isoenzyme type 2 (11-b HSD2) enzyme. We conducted a systematic review and meta-analysis to assess the effect of prenatal psychological distress (PPD) on placental 11-b HSD2 gene expression and explore the related mechanistic pathways involved in fetal neurodevelopment. Methods: We searched PubMed, Embase, Scopus, APA PsycInfo(r), and ProQuest Dissertations for observational studies assessing the association between PPD and 11-b HSD2 expression in human placentas. Adjusted regression coefficients (b) and corresponding 95% confidence intervals (CIs) were pooled based on three contextual PPD exposure groups: prenatal depression, anxiety symptoms, and perceived stress. Results: Of 3159 retrieved records, sixteen longitudinal studies involving 1869 participants across seven countries were included. Overall, exposure to PPD disorders showed weak negative associations with the placental 11-b HSD2 gene expression as follows: prenatal depression (b -0.01, 95% CI 0.05-0.02, I2=0%), anxiety symptoms (b -0.02, 95% CI 0.06-0.01, I2=0%), and perceived stress (b -0.01 95% CI 0.06-0.04, I2=62.8%). Third-trimester PPD exposure was more frequently associated with lower placental 11-b HSD2 levels. PPD and placental 11-b HSD2 were associated with changes in cortisol reactivity and the development of adverse health outcomes in mothers and children. Female-offspring were more vulnerable to PPD exposures. Conclusion: The study presents evidence of a modest role of prenatal psychological distress in regulating placental 11-b HSD2 gene expression. Future prospective cohorts utilizing larger sample sizes or advanced statistical methods to enhance the detection of small effect sizes should be planned. Additionally, controlling for key predictors such as the mother's ethnicity, trimester of PPD exposure, mode of delivery, and infant sex is crucial for valid exploration of PPD effects on fetal programming. (PsycInfo Database Record (c) 2024 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -3618,7 +3618,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>maternal outcomes using delayed pushing versus immediate pushing in the second stage of labour: an umbrella review;2024;deusa-lópez</t>
+          <t>maternaloutcomesusingdelayedpushingversusimmediatepushinginthesecondstageoflabour:anumbrellareview;2024;deusa-lopez</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Deusa-López, Paula;Cuenca-Martínez, Ferran;Sánchez-Martínez, Vanessa;Sempere-Rubio, Núria</t>
+          <t>Deusa-Lopez, Paula;Cuenca-Martinez, Ferran;Sanchez-Martinez, Vanessa;Sempere-Rubio, Nuria</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -3667,14 +3667,14 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Deusa-López</t>
+          <t>Deusa-Lopez</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>the impact of telehealth applications on pregnancy outcomes and costs in high-risk pregnancy: a systematic review and meta-analysis;2024;güneş öztürk</t>
+          <t>theimpactoftelehealthapplicationsonpregnancyoutcomesandcostsinhigh-riskpregnancy:asystematicreviewandmeta-analysis;2024;gunesozturk</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3687,12 +3687,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Güneş Öztürk, Gizem;Akyıldız, Deniz;Karaçam, Zekiye</t>
+          <t>Gunes Ozturk, Gizem;Akyildiz, Deniz;Karacam, Zekiye</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Introduction: Telehealth is an applicable, acceptable, cost-effective, easily accessible, and speedy method for pregnant women. This study aimed to examine the impact of telehealth applications on pregnancy outcomes and costs in highrisk pregnancies. Methods: Studies were selected from PubMed, Science Direct, Web of Science, EBSCO, Scopus, and Clinical Key databases according to the inclusion and exclusion criteria from January to February 2021. Cochrane risk-of-bias tools were used in the quality assessment of the studies. Results: Four observational and eight randomized controlled studies were included in this meta-analysis (telehealth: 135,875, control: 94,275). It was seen that the number of ultrasound (p &lt; 0.01) and face-to-face visits (p &lt; 0.01), fasting insulin (p &lt; 0.01), hemoglobin A1C before delivery (p &lt; 0.01), and emergency cesarean section rates (p = 0.05) were lower in the telehealth group. In the telehealth group, the women’s use of antenatal corticosteroids (p = 0.03) and hypoglycemic medication at delivery (p = 0.03), the total of nursing interventions (p &lt; 0.01), compliance with actual blood glucose measurements (p &lt; 0.01), induction intervention at delivery (p = 0.003), and maternal mortality (p &lt; 0.001) rates were higher. Two groups were similar in terms of the use of medical therapy, total gestational weight gain, health problems related to pregnancy, mode and complications of delivery, maternal intensive care unit admission, fetal-neonatal growth and development, neonatal health problems and mortality, follow-up, and care costs. Discussion: Telehealth and routine care yielded similar maternal/neonatal health and cost outcomes. It can be said that telehealth is a safe technique to work with in the management of high-risk pregnancies. (PsycInfo Database Record (c) 2024 APA, all rights reserved)</t>
+          <t>Introduction: Telehealth is an applicable, acceptable, cost-effective, easily accessible, and speedy method for pregnant women. This study aimed to examine the impact of telehealth applications on pregnancy outcomes and costs in highrisk pregnancies. Methods: Studies were selected from PubMed, Science Direct, Web of Science, EBSCO, Scopus, and Clinical Key databases according to the inclusion and exclusion criteria from January to February 2021. Cochrane risk-of-bias tools were used in the quality assessment of the studies. Results: Four observational and eight randomized controlled studies were included in this meta-analysis (telehealth: 135,875, control: 94,275). It was seen that the number of ultrasound (p &lt; 0.01) and face-to-face visits (p &lt; 0.01), fasting insulin (p &lt; 0.01), hemoglobin A1C before delivery (p &lt; 0.01), and emergency cesarean section rates (p = 0.05) were lower in the telehealth group. In the telehealth group, the women's use of antenatal corticosteroids (p = 0.03) and hypoglycemic medication at delivery (p = 0.03), the total of nursing interventions (p &lt; 0.01), compliance with actual blood glucose measurements (p &lt; 0.01), induction intervention at delivery (p = 0.003), and maternal mortality (p &lt; 0.001) rates were higher. Two groups were similar in terms of the use of medical therapy, total gestational weight gain, health problems related to pregnancy, mode and complications of delivery, maternal intensive care unit admission, fetal-neonatal growth and development, neonatal health problems and mortality, follow-up, and care costs. Discussion: Telehealth and routine care yielded similar maternal/neonatal health and cost outcomes. It can be said that telehealth is a safe technique to work with in the management of high-risk pregnancies. (PsycInfo Database Record (c) 2024 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -3723,14 +3723,14 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Güneş Öztürk</t>
+          <t>Gunes Ozturk</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>sexual function after childbirth: a meta-analysis based on mode of delivery;2023;alimi</t>
+          <t>sexualfunctionafterchildbirth:ameta-analysisbasedonmodeofdelivery;2023;alimi</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3748,7 +3748,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Although many women report sexual dysfunction in the postpartum period, controversial research has been reported the relationship between delivery mode and sexual function. This meta-analysis aimed to investigate the sexual function after childbirth and identify the difference of sexual function based on the female sexual function index (FSFI) questionnaire in women with elective cesarean section, vaginal delivery with episiotomy and vaginal delivery without episiotomy. Studies were found by searching in Medline, PubMed, Web of Science, Scopus and considering the references of the related papers from their start dates until September 2021. All observational studies in English that reported the mean and SD of score of sexual function and its domains based on the mode of delivery were included in this meta-analysis. Random effect model was used to combine the results of included studies on female sexual function and its subdomains. Finally, 17 articles with a total population of 3410 were included in the meta-analysis. Total mean (95 percent CI) of sexual function was 24.27 (22.82, 25.72) with substantial heterogeneity among studies (χ² = 7487.63, P &lt; .001; I² = 99.45). In subgroup analyses, the mean score of sexual function was significantly differed in terms of time elapsed since delivery (P = .04) and studied country (P &lt; .001). But, the mode of delivery has no significant effect on postpartum sexual function and subdomains. The result indicated that elective cesarean section, vaginal delivery with episiotomy, vaginal delivery without episiotomy are not associated with the female sexual function. (PsycInfo Database Record (c) 2023 APA, all rights reserved)</t>
+          <t>Although many women report sexual dysfunction in the postpartum period, controversial research has been reported the relationship between delivery mode and sexual function. This meta-analysis aimed to investigate the sexual function after childbirth and identify the difference of sexual function based on the female sexual function index (FSFI) questionnaire in women with elective cesarean section, vaginal delivery with episiotomy and vaginal delivery without episiotomy. Studies were found by searching in Medline, PubMed, Web of Science, Scopus and considering the references of the related papers from their start dates until September 2021. All observational studies in English that reported the mean and SD of score of sexual function and its domains based on the mode of delivery were included in this meta-analysis. Random effect model was used to combine the results of included studies on female sexual function and its subdomains. Finally, 17 articles with a total population of 3410 were included in the meta-analysis. Total mean (95 percent CI) of sexual function was 24.27 (22.82, 25.72) with substantial heterogeneity among studies (kh2 = 7487.63, P &lt; .001; I2 = 99.45). In subgroup analyses, the mean score of sexual function was significantly differed in terms of time elapsed since delivery (P = .04) and studied country (P &lt; .001). But, the mode of delivery has no significant effect on postpartum sexual function and subdomains. The result indicated that elective cesarean section, vaginal delivery with episiotomy, vaginal delivery without episiotomy are not associated with the female sexual function. (PsycInfo Database Record (c) 2023 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>effects of ketamine and esketamine on preventing postpartum depression after cesarean delivery: a meta-analysis;2024;li</t>
+          <t>effectsofketamineandesketamineonpreventingpostpartumdepressionaftercesareandelivery:ameta-analysis;2024;li</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3846,7 +3846,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>environmental factors associated with autism spectrum disorder in southern europe: a systematic review;2023;kazantzidou</t>
+          <t>environmentalfactorsassociatedwithautismspectrumdisorderinsoutherneurope:asystematicreview;2023;kazantzidou</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3902,7 +3902,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>use of swedish smokeless tobacco during pregnancy: a systematic review of pregnancy and early life health risk;2023;brinchmann</t>
+          <t>useofswedishsmokelesstobaccoduringpregnancy:asystematicreviewofpregnancyandearlylifehealthrisk;2023;brinchmann</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3915,7 +3915,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Brinchmann, Bendik, C.;Vist, Gunn, E.;Becher, Rune;Grimsrud, Tom, K.;Elvsaas, Ida‐Kristin, Ørjasæter;Underland, Vigdis;Holme, Jørn, A.;Carlsen, Karin C., Lødrup;Kreyberg, Ina;Nordhagen, Live, S.;Bains, Karen Eline, Stensby;Carlsen, Kai‐Håkon;Alexander, Jan;Valen, Håkon</t>
+          <t>Brinchmann, Bendik, C.;Vist, Gunn, E.;Becher, Rune;Grimsrud, Tom, K.;Elvsaas, Ida-Kristin, Orjasaeter;Underland, Vigdis;Holme, Jorn, A.;Carlsen, Karin C., Lodrup;Kreyberg, Ina;Nordhagen, Live, S.;Bains, Karen Eline, Stensby;Carlsen, Kai-Hakon;Alexander, Jan;Valen, Hakon</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -3960,7 +3960,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>risk factors of postpartum depression and depressive symptoms: umbrella review of current evidence from systematic reviews and meta-analyses of observational studies;2022;gastaldon</t>
+          <t>riskfactorsofpostpartumdepressionanddepressivesymptoms:umbrellareviewofcurrentevidencefromsystematicreviewsandmeta-analysesofobservationalstudies;2022;gastaldon</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3978,7 +3978,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Background: Evidence on risk factors for postpartum depression (PPD) are fragmented and inconsistent. Aims To assess the strength and credibility of evidence on risk factors of PPD, ranking them based on the umbrella review methodology. Method: Databases were searched until 1 December 2020, for systematic reviews and meta-analyses of observational studies. Two reviewers assessed quality, credibility of associations according to umbrella review criteria (URC) and evidence certainty according to Grading of Recommendations-Assessment-Development-Evaluations criteria. Results: Including 185 observational studies (n = 3 272 093) from 11 systematic reviews, the association between premenstrual syndrome and PPD was the strongest (highly suggestive: odds ratio 2.20, 95%CI 1.81–2.68), followed by violent experiences (highly suggestive: odds ratio (OR) = 2.07, 95%CI 1.70–2.50) and unintended pregnancy (highly suggestive: OR=1.53, 95%CI 1.35–1.75). Following URC, the association was suggestive for Caesarean section (OR = 1.29, 95%CI 1.17–1.43), gestational diabetes (OR = 1.60, 95%CI 1.25–2.06) and 5-HTTPRL polymorphism (OR = 0.70, 95%CI 0.57–0.86); and weak for preterm delivery (OR = 2.12, 95%CI 1.43–3.14), anaemia during pregnancy (OR = 1.47, 95%CI 1.17–1.84), vitamin D deficiency (OR = 3.67, 95%CI 1.72–7.85) and postpartum anaemia (OR = 1.75, 95%CI 1.18–2.60). No significant associations were found for medically assisted conception and intra-labour epidural analgesia. No association was rated as ‘convincing evidence’. According to GRADE, the certainty of the evidence was low for Caesarean section, preterm delivery, 5-HTTLPR polymorphism and anaemia during pregnancy, and ‘very low’ for remaining factors. Conclusions: The most robust risk factors of PDD were premenstrual syndrome, violent experiences and unintended pregnancy. These results should be integrated in clinical algorithms to assess the risk of PPD. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
+          <t>Background: Evidence on risk factors for postpartum depression (PPD) are fragmented and inconsistent. Aims To assess the strength and credibility of evidence on risk factors of PPD, ranking them based on the umbrella review methodology. Method: Databases were searched until 1 December 2020, for systematic reviews and meta-analyses of observational studies. Two reviewers assessed quality, credibility of associations according to umbrella review criteria (URC) and evidence certainty according to Grading of Recommendations-Assessment-Development-Evaluations criteria. Results: Including 185 observational studies (n = 3 272 093) from 11 systematic reviews, the association between premenstrual syndrome and PPD was the strongest (highly suggestive: odds ratio 2.20, 95%CI 1.81-2.68), followed by violent experiences (highly suggestive: odds ratio (OR) = 2.07, 95%CI 1.70-2.50) and unintended pregnancy (highly suggestive: OR=1.53, 95%CI 1.35-1.75). Following URC, the association was suggestive for Caesarean section (OR = 1.29, 95%CI 1.17-1.43), gestational diabetes (OR = 1.60, 95%CI 1.25-2.06) and 5-HTTPRL polymorphism (OR = 0.70, 95%CI 0.57-0.86); and weak for preterm delivery (OR = 2.12, 95%CI 1.43-3.14), anaemia during pregnancy (OR = 1.47, 95%CI 1.17-1.84), vitamin D deficiency (OR = 3.67, 95%CI 1.72-7.85) and postpartum anaemia (OR = 1.75, 95%CI 1.18-2.60). No significant associations were found for medically assisted conception and intra-labour epidural analgesia. No association was rated as 'convincing evidence'. According to GRADE, the certainty of the evidence was low for Caesarean section, preterm delivery, 5-HTTLPR polymorphism and anaemia during pregnancy, and 'very low' for remaining factors. Conclusions: The most robust risk factors of PDD were premenstrual syndrome, violent experiences and unintended pregnancy. These results should be integrated in clinical algorithms to assess the risk of PPD. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -4016,12 +4016,12 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>postpartum hemorrhage and postpartum depression: a systematic review and meta‐analysis of observational studies;2023;schoretsanitis</t>
+          <t>postpartumhemorrhageandpostpartumdepression:asystematicreviewandmeta-analysisofobservationalstudies;2023;schoretsanitis</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>postpartum hemorrhage and postpartum depression: a systematic review and meta‐analysis of observational studies</t>
+          <t>postpartum hemorrhage and postpartum depression: a systematic review and meta-analysis of observational studies</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -4029,12 +4029,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Schoretsanitis, Georgios;Gastaldon, Chiara;Ochsenbein‐Koelble, Nicole;Olbrich, Sebastian;Barbui, Corrado;Seifritz, Erich</t>
+          <t>Schoretsanitis, Georgios;Gastaldon, Chiara;Ochsenbein-Koelble, Nicole;Olbrich, Sebastian;Barbui, Corrado;Seifritz, Erich</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Objective To assess the postpartum depression (PPD) risk in women with postpartum hemorrhage (PPH) and moderators. Methods We identified observational studies of PPD rates in women with versus without PPH in Embase/Medline/PsychInfo/Cinhail in 09/2022. Study quality was evaluated using the Newcastle‐Ottawa‐Scale. Our primary outcome was the odds ratio (OR, 95% confidence intervals [95%CI]) of PPD in women with versus without PPH. Meta‐regression analyses included the effects of age, body mass index, marital status, education, history of depression/anxiety, preeclampsia, antenatal anemia and C‐section; subgroup analyses were based on PPH and PPD assessment methods, samples with versus without history of depression/anxiety, from low‐/middle‐ versus high‐income countries. We performed sensitivity analyses after excluding poor‐quality studies, cross‐sectional studies and sequentially each study. Results One, five and three studies were rated as good‐, fair‐ and poor‐quality respectively. In nine studies (k = 10 cohorts, n = 934,432), women with PPH were at increased PPD risk compared to women without PPH (OR = 1.28, 95% CI = 1.13 to 1.44, p &lt; 0.001), with substantial heterogeneity (I2 = 98.9%). Higher PPH‐related PPD ORs were estimated in samples with versus without history of depression/anxiety or antidepressant exposure (OR = 1.37, 95%CI = 1.18 to 1.60, k = 6, n = 55,212, versus 1.06, 95%CI = 1.04 to 1.09, k = 3, n = 879,220, p &lt; 0.001) and in cohorts from low‐/middle‐ versus high‐income countries (OR = 1.49, 95%CI = 1.37 to 1.61, k = 4, n = 9197, versus 1.13, 95%CI = 1.04 to 1.23, k = 6, n = 925,235, p &lt; 0.001). After excluding low‐quality studies the PPD OR dropped (1.14, 95%CI = 1.02 to 1.29, k = 6, n = 929,671, p = 0.02). Conclusions Women with PPH had increased PPD risk amplified by history of depression/anxiety, whereas more data from low‐/middle‐income countries are required. (PsycInfo Database Record (c) 2023 APA, all rights reserved)</t>
+          <t>Objective To assess the postpartum depression (PPD) risk in women with postpartum hemorrhage (PPH) and moderators. Methods We identified observational studies of PPD rates in women with versus without PPH in Embase/Medline/PsychInfo/Cinhail in 09/2022. Study quality was evaluated using the Newcastle-Ottawa-Scale. Our primary outcome was the odds ratio (OR, 95% confidence intervals [95%CI]) of PPD in women with versus without PPH. Meta-regression analyses included the effects of age, body mass index, marital status, education, history of depression/anxiety, preeclampsia, antenatal anemia and C-section; subgroup analyses were based on PPH and PPD assessment methods, samples with versus without history of depression/anxiety, from low-/middle- versus high-income countries. We performed sensitivity analyses after excluding poor-quality studies, cross-sectional studies and sequentially each study. Results One, five and three studies were rated as good-, fair- and poor-quality respectively. In nine studies (k = 10 cohorts, n = 934,432), women with PPH were at increased PPD risk compared to women without PPH (OR = 1.28, 95% CI = 1.13 to 1.44, p &lt; 0.001), with substantial heterogeneity (I2 = 98.9%). Higher PPH-related PPD ORs were estimated in samples with versus without history of depression/anxiety or antidepressant exposure (OR = 1.37, 95%CI = 1.18 to 1.60, k = 6, n = 55,212, versus 1.06, 95%CI = 1.04 to 1.09, k = 3, n = 879,220, p &lt; 0.001) and in cohorts from low-/middle- versus high-income countries (OR = 1.49, 95%CI = 1.37 to 1.61, k = 4, n = 9197, versus 1.13, 95%CI = 1.04 to 1.23, k = 6, n = 925,235, p &lt; 0.001). After excluding low-quality studies the PPD OR dropped (1.14, 95%CI = 1.02 to 1.29, k = 6, n = 929,671, p = 0.02). Conclusions Women with PPH had increased PPD risk amplified by history of depression/anxiety, whereas more data from low-/middle-income countries are required. (PsycInfo Database Record (c) 2023 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -4074,7 +4074,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>polycystic ovary syndrome and postpartum depression: a systematic review and meta-analysis of observational studies;2022;schoretsanitis</t>
+          <t>polycysticovarysyndromeandpostpartumdepression:asystematicreviewandmeta-analysisofobservationalstudies;2022;schoretsanitis</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4092,7 +4092,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Objective: To estimate the risk of postpartum depression (PPD) in women with polycystic ovary syndrome (PCOS) and assess related moderators. Methods: Observational studies reporting on PPD rates in women with vs. without PCOS were identified in Embase/Medline/PsychInfo/Cinhail in 03/2021 since data inception. Quality of studies was evaluated using the Newcastle-Ottawa-Scale. The primary outcome was the odds ratio (OR, 95% confidence intervals [95%CI]) of PPD in women with vs. without PCOS. Meta-regression analyses included the effects of age, body mass index, percent smokers, history of depression, preterm delivery, hypertension during pregnancy, gestational diabetes and cesarian section as well as subgroup analyses based on the assessment methods for PCOS and PPD. Sensitivity analyses after excluding poor quality studies and cross-sectional studies and sequentially excluding each study were performed. Results: One study was rated as good, two as fair and three as low-quality. In six studies (n = 934,922), 44,167 women with PCOS were at increased PPD risk compared to 890,755 women without PCOS (OR = 1.45, 95%CI = 1.18 to 1.79, p &lt; 0.001). When excluding one study that underestimated PCOS prevalence, we estimated an OR of 1.59 (95%CI = 1.56 to 1.62, p &lt; 0.001) with reduced heterogeneity (I² = 45.3%). Higher ORs of PPD in women with PCOS were moderated by lower percentage of preterm delivery (co-efficient -0.07, 95%CI = -0.1 to -0.04, p &lt; 0.001). After excluding low-quality studies yielded an OR of 1.58 (95%CI = 1.56 to 1.59, p &lt; 0.001) with heterogeneity dropping (I² = 14.0%). Limitations: The methodological heterogeneity of available studies. Conclusions: Women with PCOS are at elevated PPD risk with risk moderators requiring further research. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
+          <t>Objective: To estimate the risk of postpartum depression (PPD) in women with polycystic ovary syndrome (PCOS) and assess related moderators. Methods: Observational studies reporting on PPD rates in women with vs. without PCOS were identified in Embase/Medline/PsychInfo/Cinhail in 03/2021 since data inception. Quality of studies was evaluated using the Newcastle-Ottawa-Scale. The primary outcome was the odds ratio (OR, 95% confidence intervals [95%CI]) of PPD in women with vs. without PCOS. Meta-regression analyses included the effects of age, body mass index, percent smokers, history of depression, preterm delivery, hypertension during pregnancy, gestational diabetes and cesarian section as well as subgroup analyses based on the assessment methods for PCOS and PPD. Sensitivity analyses after excluding poor quality studies and cross-sectional studies and sequentially excluding each study were performed. Results: One study was rated as good, two as fair and three as low-quality. In six studies (n = 934,922), 44,167 women with PCOS were at increased PPD risk compared to 890,755 women without PCOS (OR = 1.45, 95%CI = 1.18 to 1.79, p &lt; 0.001). When excluding one study that underestimated PCOS prevalence, we estimated an OR of 1.59 (95%CI = 1.56 to 1.62, p &lt; 0.001) with reduced heterogeneity (I2 = 45.3%). Higher ORs of PPD in women with PCOS were moderated by lower percentage of preterm delivery (co-efficient -0.07, 95%CI = -0.1 to -0.04, p &lt; 0.001). After excluding low-quality studies yielded an OR of 1.58 (95%CI = 1.56 to 1.59, p &lt; 0.001) with heterogeneity dropping (I2 = 14.0%). Limitations: The methodological heterogeneity of available studies. Conclusions: Women with PCOS are at elevated PPD risk with risk moderators requiring further research. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -4130,12 +4130,12 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>risk factors for severe perineal lacerations during childbirth: a systematic review and meta‐analysis of cohort studies;2022;hu</t>
+          <t>riskfactorsforsevereperineallacerationsduringchildbirth:asystematicreviewandmeta-analysisofcohortstudies;2022;hu</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>risk factors for severe perineal lacerations during childbirth: a systematic review and meta‐analysis of cohort studies</t>
+          <t>risk factors for severe perineal lacerations during childbirth: a systematic review and meta-analysis of cohort studies</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -4148,7 +4148,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Aims and objectives To evaluate and quantify the best available evidence regarding risk factors for severe perineal lacerations. Background Many studies have evaluated the risk factors for severe perineal lacerations. However, the results of those studies are inconsistent, and meta‐analysis which thoroughly evaluates the risk factors for severe perineal lacerations is still lacking. Design Systematic review and meta‐analysis of cohort studies based on the PRISMA guideline. Methods PubMed, Embase, the Cochrane Library, CINAHL, ClinicalTrials.gov, CNKI, Wanfang Data, VIP and SinoMed were systematically searched for cohort studies reporting at least one risk factor for severe perineal lacerations from 1 January 2000 to 2 June 2021. Two reviewers independently conducted quality appraisal by NOS scale and extracted data. Data synthesis was conducted via RevMan 5.3 using a random‐effects or fixed‐effects model. Results A total of 47 studies with 7,043,218 women were included. The results showed that prior caesarean delivery (OR: 1.46, 95% CI 1.12–1.92) and pre‐pregnant underweight (OR: 1.31, 95% CI 1.22–1.41) significantly increased the risk of severe perineal lacerations. The results also demonstrated that episiotomy was protective against severe perineal lacerations in forceps delivery (OR: 0.56, 95% CI 0.42–0.74), but not spontaneous vaginal delivery (OR: 1.30, 95% CI 0.81–2.07) or vacuum delivery (OR: 0.76, 95% CI 0.45–1.28). Nulliparity, foetus in occipitoposterior or occipitotransverse position, and midline episiotomy were also independent risk factors for severe perineal lacerations. Conclusions Severe perineal lacerations are associated with many factors, and evidence‐based risk assessment tools are needed to guide the midwives and obstetricians to estimate women's risk of severe perineal lacerations. Relevance to clinical practice This systematic review and meta‐analysis identified some important risk factors for severe perineal lacerations, which provides comprehensive insights to guide the midwives to assess women's risk for severe perineal lacerations and take appropriate preventive measures to decrease the risk. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
+          <t>Aims and objectives To evaluate and quantify the best available evidence regarding risk factors for severe perineal lacerations. Background Many studies have evaluated the risk factors for severe perineal lacerations. However, the results of those studies are inconsistent, and meta-analysis which thoroughly evaluates the risk factors for severe perineal lacerations is still lacking. Design Systematic review and meta-analysis of cohort studies based on the PRISMA guideline. Methods PubMed, Embase, the Cochrane Library, CINAHL, ClinicalTrials.gov, CNKI, Wanfang Data, VIP and SinoMed were systematically searched for cohort studies reporting at least one risk factor for severe perineal lacerations from 1 January 2000 to 2 June 2021. Two reviewers independently conducted quality appraisal by NOS scale and extracted data. Data synthesis was conducted via RevMan 5.3 using a random-effects or fixed-effects model. Results A total of 47 studies with 7,043,218 women were included. The results showed that prior caesarean delivery (OR: 1.46, 95% CI 1.12-1.92) and pre-pregnant underweight (OR: 1.31, 95% CI 1.22-1.41) significantly increased the risk of severe perineal lacerations. The results also demonstrated that episiotomy was protective against severe perineal lacerations in forceps delivery (OR: 0.56, 95% CI 0.42-0.74), but not spontaneous vaginal delivery (OR: 1.30, 95% CI 0.81-2.07) or vacuum delivery (OR: 0.76, 95% CI 0.45-1.28). Nulliparity, foetus in occipitoposterior or occipitotransverse position, and midline episiotomy were also independent risk factors for severe perineal lacerations. Conclusions Severe perineal lacerations are associated with many factors, and evidence-based risk assessment tools are needed to guide the midwives and obstetricians to estimate women's risk of severe perineal lacerations. Relevance to clinical practice This systematic review and meta-analysis identified some important risk factors for severe perineal lacerations, which provides comprehensive insights to guide the midwives to assess women's risk for severe perineal lacerations and take appropriate preventive measures to decrease the risk. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -4186,7 +4186,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>the association of birth by caesarean section and cognitive outcomes in offspring: a systematic review;2021;blake</t>
+          <t>theassociationofbirthbycaesareansectionandcognitiveoutcomesinoffspring:asystematicreview;2021;blake</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -4204,7 +4204,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Purpose: Studies have reported children born by caesarean section are more likely to have lower cognitive outcomes compared to those born by vaginal delivery. This paper reviews the literature examining caesarean birth and offspring cognitive outcomes. Methods: A systematic search for observational studies or case–control studies that compared cognitive outcomes of people born by caesarean section with those born by vaginal delivery was conducted in six databases (Medline, PubMed, EMBASE, PsychInfo, CINAHL, Web of Science) from inception until December 2019 according to the Preferred Reporting Items for Systematic Reviews and Meta-Analyses (PRISMA) guidelines. Studies were assessed for quality and a narrative synthesis was undertaken considering the evidence for a causal relationship according to the Bradford Hill Criteria. Results: A total of seven studies were identified. Of these, four found a significant association between elective and emergency caesarean birth and reduction in offspring cognitive performance as measured by school performance or validated cognitive testing. Three studies found no association. There was variability in the quality of the studies, assessment of the reason for caesarean section (emergency vs elective), measurement of outcomes and adjustment for confounding factors. Conclusion: The evidence of an association between CS birth and lower offspring cognitive functioning is inconsistent. Based on currently available data, there is no evidence that a causal association exists. To better examine this association, future studies should (a) distinguish elective and emergency caesareans, (b) adequately adjust for confounding variables and (c) have valid outcome measures of cognition. (PsycInfo Database Record (c) 2023 APA, all rights reserved)</t>
+          <t>Purpose: Studies have reported children born by caesarean section are more likely to have lower cognitive outcomes compared to those born by vaginal delivery. This paper reviews the literature examining caesarean birth and offspring cognitive outcomes. Methods: A systematic search for observational studies or case-control studies that compared cognitive outcomes of people born by caesarean section with those born by vaginal delivery was conducted in six databases (Medline, PubMed, EMBASE, PsychInfo, CINAHL, Web of Science) from inception until December 2019 according to the Preferred Reporting Items for Systematic Reviews and Meta-Analyses (PRISMA) guidelines. Studies were assessed for quality and a narrative synthesis was undertaken considering the evidence for a causal relationship according to the Bradford Hill Criteria. Results: A total of seven studies were identified. Of these, four found a significant association between elective and emergency caesarean birth and reduction in offspring cognitive performance as measured by school performance or validated cognitive testing. Three studies found no association. There was variability in the quality of the studies, assessment of the reason for caesarean section (emergency vs elective), measurement of outcomes and adjustment for confounding factors. Conclusion: The evidence of an association between CS birth and lower offspring cognitive functioning is inconsistent. Based on currently available data, there is no evidence that a causal association exists. To better examine this association, future studies should (a) distinguish elective and emergency caesareans, (b) adequately adjust for confounding variables and (c) have valid outcome measures of cognition. (PsycInfo Database Record (c) 2023 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -4244,12 +4244,12 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>risk factors for neonatal brachial plexus palsy: a systematic review and meta‐analysis;2020;van der looven</t>
+          <t>riskfactorsforneonatalbrachialplexuspalsy:asystematicreviewandmeta-analysis;2020;vanderlooven</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>risk factors for neonatal brachial plexus palsy: a systematic review and meta‐analysis</t>
+          <t>risk factors for neonatal brachial plexus palsy: a systematic review and meta-analysis</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -4262,7 +4262,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Aim: To provide a comprehensive update on the most prevalent, significant risk factors for neonatal brachial plexus palsy (NBPP). Method: Cochrane CENTRAL, MEDLINE, Web of Science, Embase, and ClinicalTrials.gov were searched for relevant publications up to March 2019. Studies assessing risk factors of NBPP in relation to typically developing comparison individuals were included. Meta‐analysis was performed for the five most significant risk factors, on the basis of the PRISMA statement and MOOSE guidelines. Pooled odds ratios (ORs), 95% confidence intervals (CIs), and across‐study heterogeneity (I2) were reported. Reporting bias and quality of evidence was rated. In addition, we assessed the incidence of NBPP. Results: Twenty‐two observational studies with a total sample size of 29 419 037 live births were selected. Significant risk factors included shoulder dystocia (OR 115.27; 95% CI 81.35–163.35; I² = 92%), macrosomia (OR 9.75; 95% CI 8.29–11.46; I² = 70%), (gestational) diabetes (OR 5.33; 95% CI 3.77–7.55; I² = 59%), instrumental delivery (OR 3.8; 95% CI 2.77–5.23; I² = 77%), and breech delivery (OR 2.49; 95% CI 1.67–3.7; I² = 70%). Caesarean section appeared as a protective factor (OR 0.13; 95% CI 0.11–0.16; I² = 41%). The pooled overall incidence of NBPP was 1.74 per 1000 live births. It has decreased in recent years. Interpretation: The incidence of NBPP is decreasing. Shoulder dystocia, macrosomia, maternal diabetes, instrumental delivery, and breech delivery are risk factors for NBPP. Caesarean section appears as a protective factor. What this paper adds The overall incidence of neonatal brachial plexus palsy is 1.74 per 1000 live births. The incidence has declined significantly. Shoulder dystocia, macrosomia, maternal diabetes, instrumental delivery, and breech delivery are the main risk factors. Prevention is difficult owing to unpredictability and often labour‐related risk. (PsycInfo Database Record (c) 2020 APA, all rights reserved)</t>
+          <t>Aim: To provide a comprehensive update on the most prevalent, significant risk factors for neonatal brachial plexus palsy (NBPP). Method: Cochrane CENTRAL, MEDLINE, Web of Science, Embase, and ClinicalTrials.gov were searched for relevant publications up to March 2019. Studies assessing risk factors of NBPP in relation to typically developing comparison individuals were included. Meta-analysis was performed for the five most significant risk factors, on the basis of the PRISMA statement and MOOSE guidelines. Pooled odds ratios (ORs), 95% confidence intervals (CIs), and across-study heterogeneity (I2) were reported. Reporting bias and quality of evidence was rated. In addition, we assessed the incidence of NBPP. Results: Twenty-two observational studies with a total sample size of 29 419 037 live births were selected. Significant risk factors included shoulder dystocia (OR 115.27; 95% CI 81.35-163.35; I2 = 92%), macrosomia (OR 9.75; 95% CI 8.29-11.46; I2 = 70%), (gestational) diabetes (OR 5.33; 95% CI 3.77-7.55; I2 = 59%), instrumental delivery (OR 3.8; 95% CI 2.77-5.23; I2 = 77%), and breech delivery (OR 2.49; 95% CI 1.67-3.7; I2 = 70%). Caesarean section appeared as a protective factor (OR 0.13; 95% CI 0.11-0.16; I2 = 41%). The pooled overall incidence of NBPP was 1.74 per 1000 live births. It has decreased in recent years. Interpretation: The incidence of NBPP is decreasing. Shoulder dystocia, macrosomia, maternal diabetes, instrumental delivery, and breech delivery are risk factors for NBPP. Caesarean section appears as a protective factor. What this paper adds The overall incidence of neonatal brachial plexus palsy is 1.74 per 1000 live births. The incidence has declined significantly. Shoulder dystocia, macrosomia, maternal diabetes, instrumental delivery, and breech delivery are the main risk factors. Prevention is difficult owing to unpredictability and often labour-related risk. (PsycInfo Database Record (c) 2020 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -4302,12 +4302,12 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>prenatal, perinatal and neonatal risk factors for perinatal arterial ischaemic stroke: a systematic review and meta‐analysis;2017;li</t>
+          <t>prenatal,perinatalandneonatalriskfactorsforperinatalarterialischaemicstroke:asystematicreviewandmeta-analysis;2017;li</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>prenatal, perinatal and neonatal risk factors for perinatal arterial ischaemic stroke: a systematic review and meta‐analysis</t>
+          <t>prenatal, perinatal and neonatal risk factors for perinatal arterial ischaemic stroke: a systematic review and meta-analysis</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -4320,7 +4320,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>The aim of the present study was to perform a meta‐analysis of published data to determine the significance of clinical factors and exposures to the risk of perinatal arterial ischaemic stroke (PAIS) and provide guidance for clinical diagnosis and treatment. A comprehensive literature search of the PubMed, Embase, MEDLINE and Cochrane Library databases for relevant observational studies (cohort/case−control) from March 1984 to March 2016 was undertaken. Two review authors independently examined the full text records to determine which studies met the inclusion criteria and evaluated risk factors for PAIS. Risk ratios, odds ratios and 95% confidence intervals were estimated. A total of 11 studies were included in the analyses. Intrapartum fever &gt; 38°C, pre‐eclampsia, oligohydramnios, primiparity, forceps delivery, vacuum delivery, fetal heart rate abnormalities, abnormal cardiotocography tracing, cord abnormalities, birth asphyxia, emergency caesarean section, tight nuchal cord, meconium‐stained amniotic fluid, umbilical arterial pH &lt; 7.10, Apgar score at 5 min &lt; 7, resuscitation at birth, hypoglycaemia, male gender and small for gestational age were identified as risk factors for PAIS. This systemic review and meta‐analysis provides a preliminary evidence‐based assessment of the risk factors for PAIS. Patients with any of the risk factors identified in this analysis should be given careful consideration to ensure the prevention of PAIS. Future studies focusing on the combined effects of multiple prenatal, perinatal and neonatal risk factors for PAIS are warranted. (PsycINFO Database Record (c) 2017 APA, all rights reserved)</t>
+          <t>The aim of the present study was to perform a meta-analysis of published data to determine the significance of clinical factors and exposures to the risk of perinatal arterial ischaemic stroke (PAIS) and provide guidance for clinical diagnosis and treatment. A comprehensive literature search of the PubMed, Embase, MEDLINE and Cochrane Library databases for relevant observational studies (cohort/case-control) from March 1984 to March 2016 was undertaken. Two review authors independently examined the full text records to determine which studies met the inclusion criteria and evaluated risk factors for PAIS. Risk ratios, odds ratios and 95% confidence intervals were estimated. A total of 11 studies were included in the analyses. Intrapartum fever &gt; 38degC, pre-eclampsia, oligohydramnios, primiparity, forceps delivery, vacuum delivery, fetal heart rate abnormalities, abnormal cardiotocography tracing, cord abnormalities, birth asphyxia, emergency caesarean section, tight nuchal cord, meconium-stained amniotic fluid, umbilical arterial pH &lt; 7.10, Apgar score at 5 min &lt; 7, resuscitation at birth, hypoglycaemia, male gender and small for gestational age were identified as risk factors for PAIS. This systemic review and meta-analysis provides a preliminary evidence-based assessment of the risk factors for PAIS. Patients with any of the risk factors identified in this analysis should be given careful consideration to ensure the prevention of PAIS. Future studies focusing on the combined effects of multiple prenatal, perinatal and neonatal risk factors for PAIS are warranted. (PsycINFO Database Record (c) 2017 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>in-utero and perinatal influences on suicide risk: a systematic review and meta-analysis;2019;orri</t>
+          <t>in-uteroandperinatalinfluencesonsuiciderisk:asystematicreviewandmeta-analysis;2019;orri</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -4378,7 +4378,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Background: Adverse in-utero and perinatal conditions might contribute to an increased suicide risk throughout the lifespan; however, existing evidence is sparse and contradictory. We aimed to investigate in-utero and perinatal exposures associated with suicide, suicide attempt, and suicidal ideation. Methods: We did a systematic review and meta-analysis and searched MEDLINE, Embase, and PsycINFO from inception to Jan 24, 2019, for population-based prospective studies that investigated the association between in-utero and perinatal factors and suicide, suicide attempt, and suicidal ideation. Only papers published in English in peer-reviewed journals were considered. Two researchers independently extracted formal information (eg, country, year, duration of follow-up) and number of cases and non-cases exposed and non-exposed to each risk factor. We calculated pooled odds ratios (ORs) with 95% CIs using random-effects models and used meta-regression to investigate heterogeneity. This study was registered with PROSPERO, number CRD42018091205. Findings: We identified 42 eligible studies; they had a low risk of bias (median quality score 9/9 [IQR 8–9]). Family or parental characteristics, such as high birth order (eg, for fourth-born or later-born vs first-born, pooled OR 1·51 [95% CIs 1·21–1·88]), teenage mothers (1·80 [1·52–2·14]), single mothers (1·57 [1·31–1·89]); indices of socioeconomic position, such as low maternal (1·36 [1·28–1·46]) and paternal (1·38 [1·27–1·51]) education; and fetal growth (eg, low birthweight 1·30 [1·09–1·55] and small for gestational age 1·18 [1·00–1·40]) were associated with higher suicide risk. Father's age, low gestational age, obstetric characteristics (eg, caesarean section), and condition or exposure during pregnancy (eg, maternal smoking or hypertensive disease) were not associated with higher suicide risk. Similar patterns of associations were observed for suicide attempt and suicidal ideation; however, these results were based on a lower number of studies. In meta-regression, differences in length of follow-up explained most between-study heterogeneity (inital I 2 ranged from 0 to 79·5). Interpretation: These findings suggest that prenatal and perinatal characteristics are associated with increased suicide risk during the life course, supporting the developmental origin of health and diseases hypothesis for suicide. The low number of studies for some risk factors, especially for suicide attempt and ideation, leaves gaps in knowledge that need to be addressed. The mechanisms underlying the reported associations and their causal nature still remain unclear. (PsycINFO Database Record (c) 2019 APA, all rights reserved)</t>
+          <t>Background: Adverse in-utero and perinatal conditions might contribute to an increased suicide risk throughout the lifespan; however, existing evidence is sparse and contradictory. We aimed to investigate in-utero and perinatal exposures associated with suicide, suicide attempt, and suicidal ideation. Methods: We did a systematic review and meta-analysis and searched MEDLINE, Embase, and PsycINFO from inception to Jan 24, 2019, for population-based prospective studies that investigated the association between in-utero and perinatal factors and suicide, suicide attempt, and suicidal ideation. Only papers published in English in peer-reviewed journals were considered. Two researchers independently extracted formal information (eg, country, year, duration of follow-up) and number of cases and non-cases exposed and non-exposed to each risk factor. We calculated pooled odds ratios (ORs) with 95% CIs using random-effects models and used meta-regression to investigate heterogeneity. This study was registered with PROSPERO, number CRD42018091205. Findings: We identified 42 eligible studies; they had a low risk of bias (median quality score 9/9 [IQR 8-9]). Family or parental characteristics, such as high birth order (eg, for fourth-born or later-born vs first-born, pooled OR 1*51 [95% CIs 1*21-1*88]), teenage mothers (1*80 [1*52-2*14]), single mothers (1*57 [1*31-1*89]); indices of socioeconomic position, such as low maternal (1*36 [1*28-1*46]) and paternal (1*38 [1*27-1*51]) education; and fetal growth (eg, low birthweight 1*30 [1*09-1*55] and small for gestational age 1*18 [1*00-1*40]) were associated with higher suicide risk. Father's age, low gestational age, obstetric characteristics (eg, caesarean section), and condition or exposure during pregnancy (eg, maternal smoking or hypertensive disease) were not associated with higher suicide risk. Similar patterns of associations were observed for suicide attempt and suicidal ideation; however, these results were based on a lower number of studies. In meta-regression, differences in length of follow-up explained most between-study heterogeneity (inital I 2 ranged from 0 to 79*5). Interpretation: These findings suggest that prenatal and perinatal characteristics are associated with increased suicide risk during the life course, supporting the developmental origin of health and diseases hypothesis for suicide. The low number of studies for some risk factors, especially for suicide attempt and ideation, leaves gaps in knowledge that need to be addressed. The mechanisms underlying the reported associations and their causal nature still remain unclear. (PsycINFO Database Record (c) 2019 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -4418,7 +4418,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>does caesarean section affect breastfeeding practices in china? a systematic review and meta-analysis;2017;zhao</t>
+          <t>doescaesareansectionaffectbreastfeedingpracticesinchina?asystematicreviewandmeta-analysis;2017;zhao</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -4476,7 +4476,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>the impact of negative childbirth experience on future reproductive decisions: a quantitative systematic review;2018;shorey</t>
+          <t>theimpactofnegativechildbirthexperienceonfuturereproductivedecisions:aquantitativesystematicreview;2018;shorey</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -4494,7 +4494,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Aim: The aim of this study was to systematically retrieve, critique and synthesize available evidence regarding the association between negative childbirth experiences and future reproductive decisions. Background: A child’s birth is often a joyous event; however, there is a proportion of women who undergo negative childbirth experiences that have long-term implications on their reproductive decisions. Design: A systematic review of quantitative studies was undertaken using Joanna Briggs Institute’s methods. Review methods: A search was carried out in CINAHL Plus with Full Text, Embase, PsycINFO, PubMed, Scopus and Web of Science from January 1996-July 2016. Studies that fulfilled the inclusion criteria were assessed by two independent reviewers using the Joanna Briggs Institute’s Critical Appraisal Tools. Data were extracted under subheadings adapted from the institute’s data extraction forms. Results: Twelve studies, which examined either one or more influences of negative childbirth experiences, were identified. The included studies were either cohort or cross-sectional designs. Five studies observed positive associations between prior negative childbirth experiences and decisions to not have another child, three studies found positive associations between negative childbirth experiences and decisions to delay a subsequent birth and six studies concluded positive associations between negative childbirth experiences and maternal requests for caesarean section in subsequent pregnancies. Conclusion: To receive a holistic understanding on negative childbirth experiences, a suitable definition and validated measuring tools should be used to understand this phenomenon. Future studies or reviews should include a qualitative component and/or the exploration of specific factors such as cultural and regional differences that influence childbirth experiences. (PsycINFO Database Record (c) 2019 APA, all rights reserved)</t>
+          <t>Aim: The aim of this study was to systematically retrieve, critique and synthesize available evidence regarding the association between negative childbirth experiences and future reproductive decisions. Background: A child's birth is often a joyous event; however, there is a proportion of women who undergo negative childbirth experiences that have long-term implications on their reproductive decisions. Design: A systematic review of quantitative studies was undertaken using Joanna Briggs Institute's methods. Review methods: A search was carried out in CINAHL Plus with Full Text, Embase, PsycINFO, PubMed, Scopus and Web of Science from January 1996-July 2016. Studies that fulfilled the inclusion criteria were assessed by two independent reviewers using the Joanna Briggs Institute's Critical Appraisal Tools. Data were extracted under subheadings adapted from the institute's data extraction forms. Results: Twelve studies, which examined either one or more influences of negative childbirth experiences, were identified. The included studies were either cohort or cross-sectional designs. Five studies observed positive associations between prior negative childbirth experiences and decisions to not have another child, three studies found positive associations between negative childbirth experiences and decisions to delay a subsequent birth and six studies concluded positive associations between negative childbirth experiences and maternal requests for caesarean section in subsequent pregnancies. Conclusion: To receive a holistic understanding on negative childbirth experiences, a suitable definition and validated measuring tools should be used to understand this phenomenon. Future studies or reviews should include a qualitative component and/or the exploration of specific factors such as cultural and regional differences that influence childbirth experiences. (PsycINFO Database Record (c) 2019 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -4534,7 +4534,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>feeding neonates by cup: a systematic review of the literature;2016;mckinney</t>
+          <t>feedingneonatesbycup:asystematicreviewoftheliterature;2016;mckinney</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -4590,7 +4590,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>birth-related perineal trauma in low- and middle-income countries: a systematic review and meta-analysis;2019;aguiar</t>
+          <t>birth-relatedperinealtraumainlow-andmiddle-incomecountries:asystematicreviewandmeta-analysis;2019;aguiar</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -4608,7 +4608,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Introduction: Birth-related perineal trauma (BPT) is a common consequence of vaginal births. When poorly managed, BPT can result in increased morbidity and mortality due to infections, haemorrhage, and incontinence. This review aims to collect data on rates of BPT in low- and middle-income countries (LMICs), through a systematic review and meta-analysis. Methods: The following databases were searched: Medline, Embase, Latin American and Caribbean Health Sciences Literature (LILACs), and the World Health Organization (WHO) regional databases, from 2004 to 2016. Cross-sectional data on the proportion of vaginal births that resulted in episiotomy, second degree tears or obstetric anal sphincter injuries (OASI) were extracted from studies carried out in LMICs by two independent reviewers. Estimates were meta-analysed using a random effects model; results were presented by type of BPT, parity, and mode of birth. Results: Of the 1182 citations reviewed, 74 studies providing data on 334,054 births in 41 countries were included. Five studies reported outcomes of births in the community. In LMICs, the overall rates of BPT were 46% (95% CI 36–55%), 24% (95% CI 17–32%), and 1.4% (95% CI 1.2–1.7%) for episiotomies, second degree tears, and OASI, respectively. Studies were highly heterogeneous with respect to study design and population. The overall reporting quality was inadequate. Discussion: Compared to high-income settings, episiotomy rates are high in LMIC medical facilities. There is an urgent need to improve reporting of BPT in LMICs particularly with regards to births taking in community settings. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
+          <t>Introduction: Birth-related perineal trauma (BPT) is a common consequence of vaginal births. When poorly managed, BPT can result in increased morbidity and mortality due to infections, haemorrhage, and incontinence. This review aims to collect data on rates of BPT in low- and middle-income countries (LMICs), through a systematic review and meta-analysis. Methods: The following databases were searched: Medline, Embase, Latin American and Caribbean Health Sciences Literature (LILACs), and the World Health Organization (WHO) regional databases, from 2004 to 2016. Cross-sectional data on the proportion of vaginal births that resulted in episiotomy, second degree tears or obstetric anal sphincter injuries (OASI) were extracted from studies carried out in LMICs by two independent reviewers. Estimates were meta-analysed using a random effects model; results were presented by type of BPT, parity, and mode of birth. Results: Of the 1182 citations reviewed, 74 studies providing data on 334,054 births in 41 countries were included. Five studies reported outcomes of births in the community. In LMICs, the overall rates of BPT were 46% (95% CI 36-55%), 24% (95% CI 17-32%), and 1.4% (95% CI 1.2-1.7%) for episiotomies, second degree tears, and OASI, respectively. Studies were highly heterogeneous with respect to study design and population. The overall reporting quality was inadequate. Discussion: Compared to high-income settings, episiotomy rates are high in LMIC medical facilities. There is an urgent need to improve reporting of BPT in LMICs particularly with regards to births taking in community settings. (PsycInfo Database Record (c) 2022 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -4648,7 +4648,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>epilepsy in pregnancy and reproductive outcomes: a systematic review and meta-analysis;2015;viale</t>
+          <t>epilepsyinpregnancyandreproductiveoutcomes:asystematicreviewandmeta-analysis;2015;viale</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -4666,7 +4666,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Background: Antenatal care of women with epilepsy is varied. The association of epilepsy and antiepileptic drug exposure with pregnancy outcomes needs to be quantified to guide management. We did a systematic review and meta-analysis to investigate the association between epilepsy and reproductive outcomes, with or without exposure to antiepileptic drugs. Methods: We searched MEDLINE, Embase, Cochrane, AMED, and CINAHL between Jan 1, 1990, and Jan 21, 2015, with no language or regional restrictions, for observational studies of pregnant women with epilepsy, which assessed the risk of obstetric complications in the antenatal, intrapartum, or postnatal period, and any neonatal complications. We used the Newcastle-Ottawa Scale to assess the methodological quality of the included studies, risk of bias in the selection and comparability of cohorts, and outcome. We assessed the odds of maternal and fetal complications (excluding congenital malformations) by comparing pregnant women with and without epilepsy and undertook subgroup analysis based on antiepileptic drug exposure in women with epilepsy. We summarised the association as odds ratio (OR; 95% CI) using random effects meta-analysis. The PROSPERO ID of this Systematic Review's protocol is CRD42014007547. Findings: Of 7050 citations identified, 38 studies from low-income and high-income countries met our inclusion criteria (39 articles including 2 837 325 pregnancies). Women with epilepsy versus those without (2 809 984 pregnancies) had increased odds of spontaneous miscarriage (OR 1·54, 95% CI 1·02–2·32; I² = 67%), antepartum haemorrhage (1·49, 1·01–2·20; I² = 37%), post-partum haemorrhage (1·29, 1·13–1·49; I² = 41%), hypertensive disorders (1·37, 1·21–1·55; I² = 23%), induction of labour (1·67, 1·31–2·11; I² = 64%), caesarean section (1·40, 1·23–1·58; I² = 66%), any preterm birth (&lt;37 weeks of gestation; 1·16, 1·01–1·34; I² = 64%), and fetal growth restriction (1·26, 1·20–1·33; I² = 1%). The odds of early preterm birth, gestational diabetes, fetal death or stillbirth, perinatal death, or admission to neonatal intensive care unit did not differ between women with epilepsy and those without the disorder. Interpretation: A small but significant association of epilepsy, exposure to antiepileptic drugs, and adverse outcomes exists in pregnancy. This increased risk should be taken into account when counselling women with epilepsy. Funding: EBM CONNECT Collaboration. (PsycINFO Database Record (c) 2016 APA, all rights reserved)</t>
+          <t>Background: Antenatal care of women with epilepsy is varied. The association of epilepsy and antiepileptic drug exposure with pregnancy outcomes needs to be quantified to guide management. We did a systematic review and meta-analysis to investigate the association between epilepsy and reproductive outcomes, with or without exposure to antiepileptic drugs. Methods: We searched MEDLINE, Embase, Cochrane, AMED, and CINAHL between Jan 1, 1990, and Jan 21, 2015, with no language or regional restrictions, for observational studies of pregnant women with epilepsy, which assessed the risk of obstetric complications in the antenatal, intrapartum, or postnatal period, and any neonatal complications. We used the Newcastle-Ottawa Scale to assess the methodological quality of the included studies, risk of bias in the selection and comparability of cohorts, and outcome. We assessed the odds of maternal and fetal complications (excluding congenital malformations) by comparing pregnant women with and without epilepsy and undertook subgroup analysis based on antiepileptic drug exposure in women with epilepsy. We summarised the association as odds ratio (OR; 95% CI) using random effects meta-analysis. The PROSPERO ID of this Systematic Review's protocol is CRD42014007547. Findings: Of 7050 citations identified, 38 studies from low-income and high-income countries met our inclusion criteria (39 articles including 2 837 325 pregnancies). Women with epilepsy versus those without (2 809 984 pregnancies) had increased odds of spontaneous miscarriage (OR 1*54, 95% CI 1*02-2*32; I2 = 67%), antepartum haemorrhage (1*49, 1*01-2*20; I2 = 37%), post-partum haemorrhage (1*29, 1*13-1*49; I2 = 41%), hypertensive disorders (1*37, 1*21-1*55; I2 = 23%), induction of labour (1*67, 1*31-2*11; I2 = 64%), caesarean section (1*40, 1*23-1*58; I2 = 66%), any preterm birth (&lt;37 weeks of gestation; 1*16, 1*01-1*34; I2 = 64%), and fetal growth restriction (1*26, 1*20-1*33; I2 = 1%). The odds of early preterm birth, gestational diabetes, fetal death or stillbirth, perinatal death, or admission to neonatal intensive care unit did not differ between women with epilepsy and those without the disorder. Interpretation: A small but significant association of epilepsy, exposure to antiepileptic drugs, and adverse outcomes exists in pregnancy. This increased risk should be taken into account when counselling women with epilepsy. Funding: EBM CONNECT Collaboration. (PsycINFO Database Record (c) 2016 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -4706,7 +4706,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>cesarean section and risk of postpartum depression: a meta-analysis;2017;xu</t>
+          <t>cesareansectionandriskofpostpartumdepression:ameta-analysis;2017;xu</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -4724,7 +4724,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Objective: The association of cesarean section (CS) with the risk of postpartum depression (PPD) remains controversial. Therefore, we conducted a meta-analysis to explore the association between CS and the risk of PPD. Methods: A systematic literature search was performed in PubMed, Web of Science and Embase databases for relevant articles up to November 2016. Pooled odds ratios (ORs) with 95% confidence intervals (CIs) were calculated with fixed-effects model or random-effects model. Results: A total of 28 studies from 27 articles involving 532,630 participants were included in this meta-analysis. The pooled OR of the association between CS and PPD risk was 1.26 (95% CI: 1.16–1.36). In subgroup analyses stratified by study design [cohort studies: (1.25, 95% CI: 1.10–1.41); case-control studies: (1.25, 95% CI: 1.00–1.56); cross-sectional studies: (1.44, 95% CI: 1.14–1.82)] and adjustment status of complications during pregnancy [adjusted for: (1.29, 95% CI: 1.12–1.48); not-adjusted for: (1.24, 95% CI: 1.13–1.36)], the abovementioned associations remained consistent. The pooled ORs of PPD were 1.15 (95% CI: 0.92–1.43) for elective cesarean section (ElCS) and 1.47 (95% CI: 1.33–1.62) for emergency cesarean section (EmCS). Conclusion: This meta-analysis suggests that CS and EmCS increase the risk of PPD. Further evidence is needed to explore the associations between the specific types of CS and the risk of PPD. (PsycInfo Database Record (c) 2020 APA, all rights reserved)</t>
+          <t>Objective: The association of cesarean section (CS) with the risk of postpartum depression (PPD) remains controversial. Therefore, we conducted a meta-analysis to explore the association between CS and the risk of PPD. Methods: A systematic literature search was performed in PubMed, Web of Science and Embase databases for relevant articles up to November 2016. Pooled odds ratios (ORs) with 95% confidence intervals (CIs) were calculated with fixed-effects model or random-effects model. Results: A total of 28 studies from 27 articles involving 532,630 participants were included in this meta-analysis. The pooled OR of the association between CS and PPD risk was 1.26 (95% CI: 1.16-1.36). In subgroup analyses stratified by study design [cohort studies: (1.25, 95% CI: 1.10-1.41); case-control studies: (1.25, 95% CI: 1.00-1.56); cross-sectional studies: (1.44, 95% CI: 1.14-1.82)] and adjustment status of complications during pregnancy [adjusted for: (1.29, 95% CI: 1.12-1.48); not-adjusted for: (1.24, 95% CI: 1.13-1.36)], the abovementioned associations remained consistent. The pooled ORs of PPD were 1.15 (95% CI: 0.92-1.43) for elective cesarean section (ElCS) and 1.47 (95% CI: 1.33-1.62) for emergency cesarean section (EmCS). Conclusion: This meta-analysis suggests that CS and EmCS increase the risk of PPD. Further evidence is needed to explore the associations between the specific types of CS and the risk of PPD. (PsycInfo Database Record (c) 2020 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -4764,7 +4764,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>gender and birth cohort differences in adult attachment in chinese college students: a meta-analysis;2017;shu</t>
+          <t>genderandbirthcohortdifferencesinadultattachmentinchinesecollegestudents:ameta-analysis;2017;shu</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -5144,7 +5144,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>pentobarbital coma use in a pregnant patient with refractory intracranial hypertension: a case report;2022;patel</t>
+          <t>pentobarbitalcomauseinapregnantpatientwithrefractoryintracranialhypertension:acasereport;2022;patel</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -5202,7 +5202,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>potential of geographical variation analysis for realigning providers to value-based care. echo case study on lower-value indications of c-section in five european countries;2015;garcía-armesto</t>
+          <t>potentialofgeographicalvariationanalysisforrealigningproviderstovalue-basedcare.echocasestudyonlower-valueindicationsofc-sectioninfiveeuropeancountries;2015;garcia-armesto</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -5215,12 +5215,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>García-Armesto, Sandra;Angulo-Pueyo, Ester;Martínez-Lizaga, Natalia;Mateus, Céu;Joaquim, Inês;Bernal-Delgado, Enrique</t>
+          <t>Garcia-Armesto, Sandra;Angulo-Pueyo, Ester;Martinez-Lizaga, Natalia;Mateus, Ceu;Joaquim, Ines;Bernal-Delgado, Enrique</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Background: Although C-section is a highly effective procedure, literature abounds with evidence of overuse and particularly misuse, in lower-value indications such as low-risk deliveries. This study aims to quantify utilization of C-section in low-risk cases, mapping out areas showing excess-usage in each country and to estimate excess-expenditure as a proxy of the opportunity cost borne by healthcare systems. Methods: Observational, ecologic study on deliveries in 913 sub-national administrative areas of five European countries (Denmark, England, Portugal, Slovenia and Spain) from 2002 to 2009. The study includes a cross-section analysis with 2009 data and a time-trend analysis for the whole period. Main endpoints: age-standardized utilization rates of C-section in low-risk pregnancies and deliveries per 100 deliveries. Secondary endpoints: Estimated excess-cases per geographical unit of analysis in two scenarios of minimized utilization. Results: C-section is widely used in all examined countries (ranging from 19% of Slovenian deliveries to 33% of deliveries in Portugal). With the exception of Portugal, there are no systematic variations in intensity of use across areas in the same country. Cross-country comparison of lower-value C-section leaves Denmark with 10% and Portugal with 2%, the highest and lowest. Such behaviour was stable over the period of analysis. Within each country, the scattered geographical patterns of use intensity speak for local drivers playing a major role within the national trend. Conclusion: The analysis conducted suggests plenty of room for enhancing value in obstetric care and equity in women’s access to such within the countries studied. The analysis of geographical variations in lower-value care can constitute a powerful screening tool. (PsycINFO Database Record (c) 2016 APA, all rights reserved)</t>
+          <t>Background: Although C-section is a highly effective procedure, literature abounds with evidence of overuse and particularly misuse, in lower-value indications such as low-risk deliveries. This study aims to quantify utilization of C-section in low-risk cases, mapping out areas showing excess-usage in each country and to estimate excess-expenditure as a proxy of the opportunity cost borne by healthcare systems. Methods: Observational, ecologic study on deliveries in 913 sub-national administrative areas of five European countries (Denmark, England, Portugal, Slovenia and Spain) from 2002 to 2009. The study includes a cross-section analysis with 2009 data and a time-trend analysis for the whole period. Main endpoints: age-standardized utilization rates of C-section in low-risk pregnancies and deliveries per 100 deliveries. Secondary endpoints: Estimated excess-cases per geographical unit of analysis in two scenarios of minimized utilization. Results: C-section is widely used in all examined countries (ranging from 19% of Slovenian deliveries to 33% of deliveries in Portugal). With the exception of Portugal, there are no systematic variations in intensity of use across areas in the same country. Cross-country comparison of lower-value C-section leaves Denmark with 10% and Portugal with 2%, the highest and lowest. Such behaviour was stable over the period of analysis. Within each country, the scattered geographical patterns of use intensity speak for local drivers playing a major role within the national trend. Conclusion: The analysis conducted suggests plenty of room for enhancing value in obstetric care and equity in women's access to such within the countries studied. The analysis of geographical variations in lower-value care can constitute a powerful screening tool. (PsycINFO Database Record (c) 2016 APA, all rights reserved)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -5251,7 +5251,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>García-Armesto</t>
+          <t>Garcia-Armesto</t>
         </is>
       </c>
     </row>
@@ -5825,12 +5825,12 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>using grade as a framework to guide research on the sexual and reproductive health and rights (srhr) of women living with hiv—methodological opportunities and challenges;2017;siegfried</t>
+          <t>usinggradeasaframeworktoguideresearchonthesexualandreproductivehealthandrights(srhr)ofwomenlivingwithhiv--methodologicalopportunitiesandchallenges;2017;siegfried</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>using grade as a framework to guide research on the sexual and reproductive health and rights (srhr) of women living with hiv—methodological opportunities and challenges</t>
+          <t>using grade as a framework to guide research on the sexual and reproductive health and rights (srhr) of women living with hiv--methodological opportunities and challenges</t>
         </is>
       </c>
       <c r="C2" t="n">

</xml_diff>